<commit_message>
fix entry disambiguation bug
BUG FIX: When enable char, entry can't be matched to the simplified characters correctly
</commit_message>
<xml_diff>
--- a/compare-result-list.xlsx
+++ b/compare-result-list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +524,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>马仁裕</t>
+          <t>馬仁裕</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -544,7 +544,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>夫道被万物，处其中者是曰贤人；功济横流，让其先者方称君子。施之则开物成务，与广业而同归；卷之则保族宜家，垂令名于必大。是以长沙吴芮，繁祉迈于三雄；南阳贾复，贲宠隆于四七。历代已降，靡不由之。迄于我朝，则扶风公其人矣。公讳仁裕，字德宽。其先扶风人，子孙或从官于徐方，今为彭城人也。粤若万邦作乂，益有佐禹之功；因封受氏，奢有却秦之绩。公侯必复，关西靡孟起之威；文武未坠，南郡被季长之德。存乎谱牒，无俟阐扬。曾祖某、祖某，皆以卤介之气，当屯蒙之运，不履王侯之事，归全父母之邦。考某，少负雄名，为武宁军裨将。才高位下，厥用弗昭，累赠尚书右仆射。傅曰：‘有明德而不显当代，后必有兴者。’故其余庆，集于我公。惟公克禀粹灵，夙彰奇应，方娠而神贶协梦，既生而异气充庭。宗族相惊，里闾交庆。识者谓之曰：‘不意英物，复钟此儿。天将启之，马氏为不朽矣。’长而爽迈，辅以博闻；善无常师，器以虚受。及皇图中否，赤县沦灾，战国纵横，争求策士，孔门堂奥，半作家臣。公负先见之明，审择君之义。举旗沛泽，即授中涓；定难京城，仍参主簿。而上方从历试，允懋臣功，经纶艸昧，咨访遗阙。公亲侍左右，日奉谟猷，能知四国之为，且掌宾客之礼。劳无伐善，夙夜不离于公；美则归君，论议莫窥其际。出入二纪，懋肩一心。车服以庸，宠禄来假，乃升朝序，乃掌禁师，以左领军将军兼总丞相之兵卫。申令惟一，任众惟睦，推以恩信，先之勤劳。周庐既严，军事以简，考绩称最，帝用嘉之。迁检校司徒，遥兼宿州刺史。夫千骑之长，可以图功，百城之权，可以观政，中外迭处，抑惟旧章，即授楚州刺史、本州团练使。甸服之际，邦赋是繁；长淮之冲，戎寄为急。公奉扬王略，遵举诏条，人不易方，计日而治。征为右卫大将军，复领旧兵，以卫相府，董齐之略，有逾于初。明年，改右金吾大将军，以扶风县三百户为封邑。执金之职，历代雄重，绵祀虚位，公首居之。内训却非之士，外察苛留之禁，熊罴宣力，辇毂无尘。及上允膺内禅，光启建业，寺府军卫，半存旧京，委公留台右师，俾率东夏。即迁检校太保，改右天威副统军，进爵为伯。陕服从入，公有力焉。及参告类之仪，益光求旧之举。宠开幕府，遥领徐方，进封郡侯，定食千户。左辅之地，王业所基，藩屏京师，惟公攸赖，乃移使节，往镇京口。公慈惠著于郡国，威德洽于士心，由是齐人向风，稘年报政，加同中书门下平章事、庐州节度观察等使。自南北分隔，戎华交驰，合淝之郊，常制冲要，故有台阶之命，以增外梱之威。公于是谨斥候、审号令。习组练之士，则声如飙驰；严堡障之备，则势若山立。虏不敢犯，边是以宁，而察俗之方，如南徐之理。方当矢谟帷扆，薄伐关河，渡江之誓既陈，溯渭之舟已具〔一〕。呜呼!良图未展，早命不融。春秋六十有三，升元六年闰三月五日，薨于庐州公署。上省奏震悼，废朝三日，即用玄甲之数，式拟铁山之功，给于官司，临以中使。奉常以视履考祥之义，循贞心大度之美，详协公论，易名曰匡。即以其年四月七日，备卤簿仪卫，葬于庐州合淝县乡里，礼也。公娶同郡莱氏，封彭城郡君。丽秾李之华，亲采蘩之职，理内协《鹊巢》之咏，从贵有鱼轩之华。某年月日先公而逝。嗣子右弓箭库使光庭、东头供奉官光祚、合门承旨光绍，皆禀义方，无忝遗烈。家承膏粱之后，而恭顺克修；职在绮纨之间，而雅素自若。君子谓扶风公其有后乎。夫碑颂之设，有自来矣。琬琰之细既垂于苕华，盘盂之微又参于警戒。若乃道合天眷，忠存王家。累辅翼之功，而钟鼎之报网阙；享将相之赏，而带砺之誓弗渝。时无间言，没有余位。故其宗庙之纪，金石之铭，昭示来云，不可诬也。小臣不学，奉旨刊文。庶使计功称德，代远而愈信；披文相质，事久而弥芬。岘首之怀靡尽，昆吾之烈长存。呜呼哀哉!其铭曰：益作朕虞，实曰元凯，崇基缔业，明德攸在。维赵于蕃，封移族改，祚实刊山，源长巨海。因枝别代，𫌪渭来迁。导德绛帐，勤王跕鸢。流光袭祉，映后昭前。怀黄结紫，著简成编。诞发材英，肇惟明懿。鼎角膺奇，龟文履异。博容泛爱，入孝出悌。运有屯蒙，器无凝滞。爰初发迹，云从潜泉。濯缨职帜，拊冀中涓。良骥处服，忘归在弦。枢机言行，无竞维贤。缱绻从君，匪伊履屐。勤毖前殳，周旋陛戟。居国必闻，在身无择。帝爰允龤，胙乃丕绩。惟彼淮泗，疆以獯夷〔二〕。维此京浙，缵以邦畿。封淮表浙，惟惠惟威。椒兰在俗，辕辙兴思。群舒待理，猃狁孔棘。帝谓侯氏，缵服新息。式固尔猷，惠此庐国。乃陟台阶，俾藩于北。龙旗四牡，钩膺镂锡。命服有炜，光声载扬。犷狄弭耳，蚩氓向方。上仪像物，下谧飞蝗。梁木或颠，通川有逝，长城既严，哲人永瘁。像著云台，风存遐裔。辍舂尽思，瞻山殒泪。信结殊俗，悲深上旻。丹碑既刻，列鼎书勋。祁连不泯，庸器长存。丕显百代，惟子有臣。《徐公文集》卷一一。又见《全唐文》卷八八五。〔一〕恪：原作‘斥’，据《全唐文》、徐校、黄校本改。〔二〕疆：原作‘强’，据《全唐文》、徐校、李刊本改。</t>
+          <t>夫道被萬物，處其中者是曰賢人；功濟横流，讓其先者方稱君子。施之則開物成務，與廣業而同歸；卷之則保族宜家，垂令名于必大。是以長沙吴芮，繁祉邁于三雄；南陽賈復，賁寵隆于四七。歷代已降，靡不由之。迄于我朝，則扶風公其人矣。公諱仁裕，字德寬。其先扶風人，子孫或從官于徐方，今爲彭城人也。粤若萬邦作乂，益有佐禹之功；因封受氏，奢有卻秦之績。公侯必復，關西靡孟起之威；文武未墜，南郡被季長之德。存乎譜牒，無俟闡揚。曾祖某、祖某，皆以鹵介之氣，當屯蒙之運，不履王侯之事，歸全父母之邦。考某，少負雄名，爲武寧軍裨將。才高位下，厥用弗昭，累贈尚書右僕射。傳曰：‘有明德而不顯當代，後必有興者。’故其餘慶，集于我公。惟公克稟粹靈，夙彰奇應，方娠而神貺協夢，既生而異氣充庭。宗族相驚，里閭交慶。識者謂之曰：‘不意英物，復鍾此兒。天將啓之，馬氏爲不朽矣。’長而爽邁，輔以博聞；善無常師，器以虛受。及皇圖中否，赤縣淪災，戰國縱橫，爭求策士，孔門堂奧，半作家臣。公負先見之明，審擇君之義。舉旗沛澤，即授中涓；定難京城，仍參主簿。而上方從歷試，允懋臣功，經綸草昧，諮訪遺闕。公親侍左右，日奉謨猷，能知四國之爲，且掌賓客之禮。勞無伐善，夙夜不離于公；美則歸君，論議莫闚其際。出入二紀，懋肩一心。車服以庸，寵祿來假，乃升朝序，乃掌禁師，以左領軍將軍兼總丞相之兵衛。申令惟一，任衆惟睦，推以恩信，先之勤勞。周廬既嚴，軍事以簡，考績稱最，帝用嘉之。遷檢校司徒，遙兼宿州刺史。夫千騎之長，可以圖功，百城之權，可以觀政，中外迭處，抑惟舊章，即授楚州刺史、本州團練使。甸服之際，邦賦是繁；長淮之衝，戎寄爲急。公奉揚王略，遵舉詔條，人不易方，計日而治。徵爲右衛大將軍，復領舊兵，以衛相府，董齊之略，有逾于初。明年，改右金吾大將軍，以扶風縣三百戶爲封邑。執金之職，歷代雄重，綿祀虛位，公首居之。內訓卻非之士，外察苛留之禁，熊羆宣力，輦轂無塵。及上允膺內禪，光啓建業，寺府軍衛，半存舊京，委公留臺右師，俾率東夏。即遷檢校太保，改右天威副統軍，進爵爲伯。陝服從入，公有力焉。及參告類之儀，益光求舊之舉。寵開幕府，遙領徐方，進封郡侯，定食千戶。左輔之地，王業所基，藩屏京師，惟公攸賴，乃移使節，往鎮京口。公慈惠著于郡國，威德洽于士心，由是齊人向風，期年報政，加同中書門下平章事、廬州節度觀察等使。自南北分隔，戎華交馳，合淝之郊，常制衝要，故有台階之命，以增外閫之威。公于是謹斥候、審號令。習組練之士，則聲如飆馳；嚴堡障之備，則勢若山立。虜不敢犯，邊是以寧，而察俗之方，如南徐之理。方當矢謨帷扆，薄伐關河，渡江之誓既陳，泝渭之舟已具〔一〕。嗚呼!良圖未展，早命不融。春秋六十有三，昇元六年閏三月五日，薨于廬州公署。上省奏震悼，廢朝三日，即用玄甲之數，式擬鐵山之功，給于官司，臨以中使。奉常以視履考祥之義，循貞心大度之美，詳協公論，易名曰匡。即以其年四月七日，備鹵簿儀衛，葬于廬州合淝縣鄉里，禮也。公娶同郡萊氏，封彭城郡君。麗穠李之華，親采蘩之職，理內協《鵲巢》之詠，從貴有魚軒之華。某年月日先公而逝。嗣子右弓箭庫使光庭、東頭供奉官光祚、閤門承旨光紹，皆稟義方，無忝遺烈。家承膏粱之後，而恭順克修；職在綺紈之間，而雅素自若。君子謂扶風公其有後乎。夫碑頌之設，有自來矣。琬琰之細既垂于苕華，盤盂之微又參于警戒。若乃道合天眷，忠存王家。累輔翼之功，而鐘鼎之報罔闕；享將相之賞，而帶礪之誓弗渝。時無間言，沒有餘位。故其宗廟之紀，金石之銘，昭示來雲，不可誣也。小臣不學，奉旨刊文。庶使計功稱德，代遠而愈信；披文相質，事久而彌芬。峴首之懷靡盡，昆吾之烈長存。嗚呼哀哉!其銘曰：益作朕虞，實曰元凱，崇基締業，明德攸在。維趙于蕃，封移族改，祚實刊山，源長巨海。因枝別代，覛渭來遷。導德絳帳，勤王跕鳶。流光襲祉，映後昭前。懷黃結紫，著簡成編。誕發材英，肇惟明懿。鼎角膺奇，龜文履異。博容汎愛，入孝出悌。運有屯蒙，器無凝滯。爰初發跡，雲從潛泉。濯纓職幟，拊冀中涓。良驥處服，忘歸在弦。樞機言行，無競維賢。繾綣從君，匪伊履屐。勤毖前殳，周旋陛戟。居國必聞，在身無擇。帝爰允諧，胙乃丕績。惟彼淮泗，疆以獯夷〔二〕。維此京浙，纘以邦畿。封淮表浙，惟惠惟威。椒蘭在俗，轅轍興思。羣舒待理，獫狁孔棘。帝謂侯氏，纘服新息。式固爾猷，惠此廬國。乃陟台階，俾藩于北。龍旂四牡，鈎膺鏤錫。命服有煒，光聲載揚。獷狄弭耳，蚩氓嚮方。上儀像物，下謐飛蝗。梁木或顛，通川有逝，長城既嚴，哲人永瘁。像著雲臺，風存遐裔。輟舂盡思，瞻山殞淚。信結殊俗，悲深上旻。丹碑既刻，列鼎書勳。祁連不泯，庸器長存。丕顯百代，惟子有臣。《徐公文集》卷一一。又見《全唐文》卷八八五。〔一〕恪：原作‘斥’，據《全唐文》、徐校、黃校本改。〔二〕疆：原作‘彊’，據《全唐文》、徐校、李刊本改。</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -556,7 +556,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>复;通</t>
+          <t>復;通</t>
         </is>
       </c>
       <c r="P2" t="n">
@@ -572,34 +572,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4966988</t>
+          <t>4966920</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18420</v>
+        <v>154415</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>江文蔚</t>
+          <t>劉崇俊</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>君章;简</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>1</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>建安</t>
+          <t>彭城</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -608,77 +604,85 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>公讳文蔚，字君章。其先济阳考城人也。昔高阳恢若水之灵，光有万国；伯益获箕山之护，克成夏功。故其子孙，延祚丕显，茅土锡胤，圭组流光。在汉者为孝子，在宋者为忠宰，在梁者为烈将，在陈者为词臣。长城既封，淮水亦绝，辞周粟而远骛，避嬴乱而深藏，徙籍建安，世为大姓。至于我王考毗、考秦，皆以隐德清操，垂为门风。惟公嗣奕叶之贤，有生知之异，幼挺奇表，夙韬殊量。殚儒墨之秘奥，穷文史之菁英。闾里归仁，宗党称孝。于时天下未一，遐方不宁，公鄙尺𫛩之为，从黄鹄之举，类延州之观乐，同太史之探书，升名俊造，从事河洛。衰俗难佐，天壤不支。我烈祖孝高皇帝，王业始于江东，仁风被于四裔，公杖策高蹈，款关来仪。府朝肃以生风，台阁蔼其增气。署宣州观察巡官，试秘书郎，迁水部员外郎，赐绯鱼袋。王国初建，改比部员外郎，知制诰。于时天人协应，狱讼攸归，舜、禹相与言，游、夏不能措，润色之任，我则无惭。既受禅，迁主客郎中，知制诰如故。俄而真拜，仍赐金紫。今上嗣位，大礼聿修，徙公为给事中，判太常卿事。时同轨胥会，有司失职，公与司门郎中萧君俨、博士韩君熙载，协力建仪，周行翕然。由是祖功宗德之位定，大行昭名之义允，功署高庙，与天无穷。明年，拜御史中丞，矫枉持平，无所顾惮，坐廷劾宰相，其言深切，贬江州司士参军。初，国朝自王义方之后〔一〕，旷数百年，宪署之间，举无废职〔二〕，然未有危言激论如此之彰灼者也。故权右振竦，朝野喧腾，傅写弹文，为之纸贵。人心既尔，天鉴亦回，前所劾者，或免或黜，公就加江州营田副使。顷之，征为卫尉卿。俄拜右谏议大夫，充翰林学士，权知贡举。出纳密命，枢机靡失，登进造士，衡镜无私，耸禁署之清风，著春官之故事。荐贤之赏，行及于台司；曳杖之稘，奄先于朝露。春秋五十有二，保大十年八月二日卒于京师官舍。皇上痛惜，为之废朝，送死恤孤，一从公赐。有司考行，易名曰简。即以其年九月十三日，葬于某县某里之原，礼也。长子翥，秘书省正字，次子𬸣，皆早卒。今以从子翘为嗣。呜呼哀哉!公心平气和，貌古神正。雅好玄理，有方外之稘；尤善词赋，得《国风》之体。去华简礼，不以位望骄人；怜才诱善，不以威名傲物。操履坚正，靡得动摇；襟怀坦夷，初无蒂介。谪居江楚，恬然自足。孜孜色养，烝烝孝心。尝为诗云：‘屈平若遇高堂在，应不怀沙独葬鱼。’此其心也。江州节度使贾公崇，以武立功，以刚肃物，事公如师傅，亲公如兄弟。时皆服公之重名，而贤贾之乐善也。既归京，寓居公廨，无以家为。二子继亡，一恸而已。齐死生于梦觉，遗宠辱于锱铢，古之达者，何以过此。呜呼!凡我僚旧，均哀共戚。入黔娄之门梱，览伯喈之经籍。睇落日以流恸，愬秋风而沾臆。企景行于高山，勒哀词于乐石。其词曰：高阳之裔，伯益之孙。展矣君子，载大其门。爰翔爰集，乐我树檀。彯缨幕府，振藻西垣。礼仪卒获，风宪攸端。道行在时，业隆自我。英英若人，见义必果。直指烈烈，宫邻琐琐。死生以之，何适不可?允矣天鉴，明哉主恩。乃还宣室，乃入修门。从容禁署，密勿王言。得才为盛，知人则难。求尸宗伯，载善其官。人必有终，古无不死。嗟嗟若人，风流永矣。徐庶有母，邓攸无子。阙里诸生，荆州故吏。谓之何哉?啜其泣矣。秋风落木，逝水成川。昨朝飞盖，今日荒千。一丘残照，万古愁烟。素车自返，宝剑高悬。高才兮直道，共尽兮何言!《徐公文集》卷一五。又见《全唐文》卷八八五。〔一〕方：原脱，据徐校、李校补。〔二〕间举：原作‘举间’，据《全唐文》、李刊本乙。</t>
+          <t>聞夫郊圻内理，牧萬民者是曰諸侯；夷狄外攘，守四方者其惟猛士。然則安危異任，文武殊塗。故天下方爭，韓、彭、英、吳橫雕戈而震耀；羣生待理，龔、黃、寇、賈擁皂蓋以從容。及夫昭格寰區，紛綸簡册，其歸一也，代有人焉。若乃總是全謨，覃于奕葉，流光受社，潛齊累將之家，崇德計功，下視慚卿之族，古難具美，我則兼之。公諱崇俊，字德修。其先彭城人。高祖升調，補山陽淮陰尉，遂家焉，即爲縣人也。岳峻洪基，海疏遙派。陽城相土，千齡侯伯之封；沛澤中興，兩代帝王之胤。懷黃結紫，論鼎甲以盱衡；刻像圖形，誓山河而捧袂。國史家牒，披卷可知。頃者聖運中微，羣方暫擾。驪山之北，犬戎興戲水之師；踐土之庭，天子屈河陽之召。公路擁南陽之衆，僭號仲家；隗囂據隴右之圖，坐論西伯。勤王問罪，吳太祖始定揚州〔一〕；賜脤專征，昭皇帝遂加殊禮。于是揚旌北討，遷寇跡于淮濱；闢土西封，謀守臣于諸將。命我顯祖，作牧鍾離。乃固堡障之嚴，載施犬馬之備。軍無粃政，將期十萬之行；師有見糧，即聚九年之蓄。方圖大舉，已仗前殳，永年不登，未幾而歿。長山群盜，舊畏來公；西域故營〔二〕，願從班勇。復命烈考，嗣膺使符。不還渭水之兵，誓卒龍門之託。故蓼城之戰，斬獲過當；汝陰之圍，策勳居最。先〇委質，鬬充國以無由；獫狁驚蒐，射郅都而不中〔三〕。疇庸錫羨，建清淮軍以壯中權；加禮慎終，贈太尉公以光幽穸。既而鼓鼙悽愴，部曲徘徊，家有遺恩，人思世德。帝曰：‘崇俊，惟爾恭儉孝友，誠明惠和，任則中軍帥，位則文昌長。誕舉攸職，予惟汝嘉。濠梁之郊，控扼遐裔，惟乃祖金，克懋厥始，乃考仁規，克慎厥中。肆予命爾，克成厥終。往哉汝諧，無廢朕命!’公銜恤奉詔，墨絰即戎，鋪陳政經，討閲軍實，思有以光大前緒，播揚國風。初，二先公之理也，屬洛邑再遷，浚郊作梗。僞新竊據，仍延十五之期；黃武開元，始創三分之業。犬牙之地，蠆尾常搖，鋒鏑縱橫，車徒奔走。摧牙獸困，尚遙匡復之謨；赬尾魚勞，未暇綏懷之術。逮公之理也，寇皆遠遁，民佇息肩。千里風從，四方聳聽。以爲格物必在于立制也，故藝貢賦以息貪暴之端，暢刑章以拯姦宄之極。賞不虛授，罰其必行。以爲富邦必在于務本也，故使民以時，相地之利。持未熟之稻，游惰自遷；班再易之田，兼并絶倖。以爲邊寧不可以忘武備也，故遠斥堠，浚溝隍，竹與木而靡遺，膏與苫而畢給，亭障屹峙，軍聲隱然。以爲強兵必在于實王畿也，故招懷邊氓，講習戎事。游兵冀馬，俱爲無犯之容；晉勇齊雄，並集選和之下。歲揀精鋭，歸之京師。其餘庶政常經，門見戶睹，斯可略而言也。高皇帝禮均元老，寵冠列藩。受禪之初，則進上公之秩；肆類之際，則委廉使之權。言必見從，無再卻之奏；君常高枕，忘北顧之憂。皇上欽奉重熙，聿遵無改，毗倚尤重，親敬有加。初，先太尉公之薨也，西北小驚，戒嚴從便，因詔執事，移清淮軍于壽春。及是，復立定遠軍，即命公爲節度使，仍以公少子匡符尚永嘉公主。留侯操印，初躋上將之壇；帝子吹簫，即降王姬之館。禮優伯舅，望重懿親。于時公涖濠梁，十有七年矣，米鹽皆序，丞史當才，閉閤罕爭，舉烽無警。朝廷以公能光前烈，雅得邊情，清淮之師，遺風仍在，俾盛一家之美，載嚴萬里之城，改壽州刺史，充清淮軍節度使。鄧侯倏去，鷄鳴傷父老之心；長者負來，虎渡息鄉閭之患。能事畢舉，考功再期。方將建大斾以風驅，指函關而電掃。雲中鷄犬，八公之跡徒存；夢裏膏肓，二竪之妖遂作。春秋四十，保大四年夏六月十有六日薨于壽春公署。皇上剪鬚靡及，穿壁方遙。投緑沈之瓜，悲哀竟日；賜黃銀之帶，慷慨霑襟。廢朝三日，中使護葬。詔兵部侍郎李貽業持節册贈太尉，賜謚曰威。即以其年秋九月十五日，備鹵簿鼓吹，葬于濠州鍾離縣大化里之原，禮也。前夫人李氏，後夫人隴西郡君李氏，皆太師趙忠懿王女也。賴鄉仙李，即開柱史之源；參野飛龍，遂紀宗卿之籍。勳庸六鎮，時高謝氏之門；師範兩朝，室有班姬之訓。荃蘪蘭蕙，映戚里以芬芳；藻荇蘋蘩，播婦儀而昭皙。門內之理，夫人有焉。子八人：二子幼；長子節，早亡；次範，滁州刺史；次簡、次策、次霸，時未仕；次符，秘書郎。或得公之政事，或得公之兵鈐，學禮學詩，惟忠惟孝，皆推酥酪之味，咸有芝蘭之芳。所謂積善餘慶，世濟其美者也。惟公山河龍鳳，凝粹彩于神姿；緯候風雲，集淵謀于靈府。議公家之事，不以身爲；行將軍之令，每由剛克。卒祖禰之成業，可謂聿修；膺牧伯之寵章，訖無虛授。所以始終匪玷，福祿攸歸。同族之間，朱輪結軌。季父仁贍，作鎮夏口。弟崇怙、崇僖，更典晉陵。其餘將軍、列侯、中郎、校尉，銀黃照爛，光浮通德之門，珩珮陸離，響雜高陽之里。茍非自天攸相，與國無疆，其孰能與于此乎!向使享大年，敷遠略，鴻飛鵬舉，功未可量也。天命不然，能無永悼!昔者荊州從事，猶牽墮淚之悲；太宰舊寮，亦有懷鉛之請。況乎世功丕顯，揭日月以高驤；帝念惟隆，會雲龍而下濟。欲垂萬葉，可不務乎?微臣職典絲綸，詞非清潤。持赤管以承詔，拂貞珉而投刃。使蚩蚩萌隸，觀跡而長懷；眇眇來雲，披文而盡信。其銘曰：惟彼陶唐，有此冀方。自天祐之，後嗣其昌。侯遷魯縣，帝隱芒碭。猗那大族，嵩華配長。渢渢彭城，興我遐祚；顯顯山陽，著我高祖。高祖伊何?仁而不遇。慶鍾令孫，聿來用武。皇運中否，諸侯起爭，浚郊怙亂〔四〕，淮壖不庭。吳王奮發，受鉞專征。命我顯祖，守濠之城。濠城嚴峻，濠兵驍勇。顯祖帥之，羣兇振恐。將軍下世，邊烽亦聳。乃命象賢，荷時之寵。荷寵伊何?載大其功。蠢蠢梁寇，言言潁墉，是馘是俘，兵無頓鋒。爰有奇略，集于威公。威公嗣侯，不墜其訓。戎事之隙，民功是振。爲之中典，著之令問。泗上風移，京師河潤。帝曰伯舅，予嘉乃勳。捍境則武，安邦則文。乃降王姬，于爾慶門。乃改乘轅，于彼西軍。西軍何在?鎮彼衡霍。威公來思，式遏寇虐。胡馬已遠，將星俄落。百身寧贖，九原誰作?明明天子，惻愴聞鼙。歲云秋止，返斾遲遲。二藩士女，泣涕漣洏。賢侯逝矣，吾誰與歸?黯黯塗山，湯湯淮涘。駟馬悲鳴，滕公所閉。甘棠勿翦，召伯攸憩。是用刊碑，永告來裔。《徐公文集》卷一一。又見《全唐文》卷八八四。〔一〕揚：原作‘楊’，據李刊本、四庫本改。〔二〕域：原作‘城’，據《全唐文》、黃校本、李刊本改。〔三〕郅：原作‘郢’，據徐校、李刊本、四庫本改。〔四〕怙：原作‘帖’，據徐校、李刊本改。</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>15</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>比部员外郎;给事中;宣州;翰林学士;判太常卿事;水部员外郎;卫尉卿;营田副使;江州;右谏议大夫;御史中丞;知制诰;主客郎中;司士参军;江州</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>翘;秦</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
         <v>0</v>
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>10;南唐</t>
+          <t>6;唐</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4967008</t>
+          <t>4966988</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>394761</v>
+        <v>18420</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>周廷构</t>
+          <t>江文蔚</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>君章;簡</t>
+        </is>
+      </c>
       <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>建安</t>
+        </is>
+      </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>君讳廷构，字正材，洛阳人也。岐山至德，绵瓜瓞者万邦；洛宅旧都，守枌榆者百世。簪组相继，谱谍存焉。曾祖侃，太常博士。祖潜，深州乐寿县令。避乱南徙，因家广陵。考延禧，明经擢第。有吴之霸，受辟为淮南巡官，累官至户部郎中，与殷文公、游贞公同掌文翰。无禄早世，故大位不跻。君即户部第四子也。幼而岐嶷，长而笃厚，躬行孝悌，余力学文。以荫释褐，补弘文馆校书，试吏为池州司户参军，改宣州宁国县尉。烈祖在藩，乃眷旧族，闻君修谨，复有吏能，因表为黄州长史，宠以朱绂，置之府朝。及受禅，迁通事舍人。鸿业肇兴，王泽遐布，赞导之任，实寄司聪，护戎修聘，观风按狱，受命而出，动网不臧。历事两朝，任遇弥厚，赏赐既数，阶勋屡迁，而通事之任如故，盖惜其能也。保大七年，转将作少监，判四方馆事。浩穰之地，尹正为难，复以本官判江宁府事。其间监诸侯之典者十，通四方之命者三，摄州府之政者六，按枉挠之狱者四。或敷惠于新附之俗，或投身于危乱之地，本于忠而后动，忘其生而后存。元宗嘉之，以为客省使。今上嗣位，深惟旧劳，特加金紫光禄大夫、台州刺史。常御寿昌殿视事，中外之人，咸得引见，又以君为寿昌殿承宣。出为忠义军监军、泉南等州宣谕使。还，迁筠州刺史、本州团练，仍使充客省使。君以备尝艰危，复逼迟暮，恳辞繁剧，恩旨不从。丙寅岁十月二十二日，终于京师某里之官舍，春秋六十有六。诏废朝一日，赐谥曰某。明年正月日葬于某所，礼也。夫人天水县君姜氏，辅佐之勤，率由妇礼，训诲诸子，备有义方。子大理评事崇俭，太常寺奉礼郎崇素，及崇顺、崇信等，皆儒谨，且不坠其先。铉家世通旧，尝接姻娅，淡成之分，终始不渝。何以置怀，是用刊德。其铭曰：猗嗟周君，世济其名。展如之人，克嗣厥声。受任干蛊，临难忘身。居中处约，全和保真。与物皆化，万古同尘。松楸勿伐，兰菊惟新。刊石表墓，于嗟善人!《徐公文集》卷一五。又见《全唐文》卷八八五。</t>
+          <t>公諱文蔚，字君章。其先濟陽考城人也。昔高陽恢若水之靈，光有萬國；伯益獲箕山之護，克成夏功。故其子孫，延祚丕顯，茅土錫胤，圭組流光。在漢者爲孝子，在宋者爲忠宰，在梁者爲烈將，在陳者爲詞臣。長城既封，淮水亦絶，辭周粟而遠騖，避嬴亂而深藏，徙籍建安，世爲大姓。至于我王考毗、考秦，皆以隱德清操，垂爲門風。惟公嗣奕葉之賢，有生知之異，幼挺奇表，夙韜殊量。殫儒墨之秘奧，窮文史之菁英。閭里歸仁，宗黨稱孝。于時天下未一，遐方不寧，公鄙尺鷃之爲，從黃鵠之舉，類延州之觀樂，同太史之探書，升名俊造，從事河洛。衰俗難佐，天壤不支。我烈祖孝高皇帝，王業始于江東，仁風被于四裔，公杖策高蹈，款關來儀。府朝肅以生風，臺閣藹其增氣。署宣州觀察巡官，試秘書郎，遷水部員外郎，賜緋魚袋。王國初建，改比部員外郎，知制誥。于時天人協應，獄訟攸歸，舜、禹相與言，游、夏不能措，潤色之任，我則無慚。既受禪，遷主客郎中，知制誥如故。俄而真拜，仍賜金紫。今上嗣位，大禮聿修，徙公爲給事中，判太常卿事。時同軌胥會，有司失職，公與司門郎中蕭君儼、博士韓君熙載，協力建儀，周行翕然。由是祖功宗德之位定，大行昭名之義允，功署高廟，與天無窮。明年，拜御史中丞，矯枉持平，無所顧憚，坐廷劾宰相，其言深切，貶江州司士參軍。初，國朝自王義方之後〔一〕，曠數百年，憲署之間，舉無廢職〔二〕，然未有危言激論如此之彰灼者也。故權右振竦，朝野喧騰，傳寫彈文，爲之紙貴。人心既爾，天鑑亦迴，前所劾者，或免或黜，公就加江州營田副使。頃之，徵爲衛尉卿。俄拜右諫議大夫，充翰林學士，權知貢舉。出納密命，樞機靡失，登進造士，衡鏡無私，聳禁署之清風，著春官之故事。薦賢之賞，行及于台司；曳杖之期，奄先于朝露。春秋五十有二，保大十年八月二日卒于京師官舍。皇上痛惜，爲之廢朝，送死卹孤，一從公賜。有司考行，易名曰簡。即以其年九月十三日，葬于某縣某里之原，禮也。長子翥，秘書省正字，次子鶱，皆早卒。今以從子翹爲嗣。嗚呼哀哉!公心平氣和，貌古神正。雅好玄理，有方外之期；尤善詞賦，得《國風》之體。去華簡禮，不以位望驕人；憐才誘善，不以威名傲物。操履堅正，靡得動搖；襟懷坦夷，初無蒂介。謫居江楚，恬然自足。孜孜色養，烝烝孝心。嘗爲詩云：‘屈平若遇高堂在，應不懷沙獨葬魚。’此其心也。江州節度使賈公崇，以武立功，以剛肅物，事公如師傅，親公如兄弟。時皆服公之重名，而賢賈之樂善也。既歸京，寓居公廨，無以家爲。二子繼亡，一慟而已。齊死生于夢覺，遺寵辱于錙銖，古之達者，何以過此。嗚呼!凡我僚舊，均哀共戚。入黔婁之門閫，覽伯喈之經籍。睇落日以流慟，愬秋風而沾臆。企景行于高山，勒哀詞于樂石。其詞曰：高陽之裔，伯益之孫。展矣君子，載大其門。爰翔爰集，樂我樹檀。彯纓幕府，振藻西垣。禮儀卒獲，風憲攸端。道行在時，業隆自我。英英若人，見義必果。直指烈烈，宮鄰瑣瑣。死生以之，何適不可?允矣天鑑，明哉主恩。乃還宣室，乃入脩門。從容禁署，密勿王言。得才爲盛，知人則難。求尸宗伯，載善其官。人必有終，古無不死。嗟嗟若人，風流永矣。徐庶有母，鄧攸無子。闕里諸生，荊州故吏。謂之何哉?啜其泣矣。秋風落木，逝水成川。昨朝飛蓋，今日荒阡。一丘殘照，萬古愁煙。素車自返，寶劍高懸。高才兮直道，共盡兮何言!《徐公文集》卷一五。又見《全唐文》卷八八五。〔一〕方：原脫，據徐校、李校補。〔二〕間舉：原作‘舉間’，據《全唐文》、李刊本乙。</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>比部員外郎;給事中;宣州;翰林學士;判太常卿事;水部員外郎;衛尉卿;營田副使;江州;右諫議大夫;御史中丞;知制誥;主客郎中;司士參軍;江州</t>
+        </is>
+      </c>
       <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>翹;秦</t>
+        </is>
+      </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
@@ -692,39 +696,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4967037</t>
+          <t>4966988</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>32565</v>
+        <v>447386</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>苗延禄</t>
+          <t>江文蔚</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>盱眙</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>公讳延禄，字世功。其先上党人。昔者楚多淫刑，贲始逃难；晋赖谋主，苗受其封。高门之庆，雄视栾、郤。绵绵瓜瓞，翼翼孙谋，存诸简编，可以扬榷。延洪于我七代祖中书舍人延嗣，光大于我六代祖太师晋卿。源流繁衍，蔚为甲族。中朝丧乱，后裔播迁，匿迹淮楚之间，今为盱眙人也。先公讳邻，生于兵戈之间，长习鼓旗之用。遭遇英主，建功立事，出为泗州防御使，入为静江军统军。世卿之祀，衰而复振。公即静江之长子也。弱不好弄，壮而有立。负雄勇之量，不以骄人；秉刚直之姿，未尝忤物。持重善战，默识寡言，时辈推之，以为君子。初，先公奉王略，领偏师，南破山越，西定江楚，东绝沧海，北捍徐戎，弓不解弮，兵不匣刃。公年甫弱冠，实参其间，搴旗斩将，所向披靡，宣力用于君父，舒壮气于风云。然而职以序迁，盖归美于先公也。烈祖孝高皇帝中兴大业，畴咨旧人，命公领泗上精兵，入为宣威军裨将。六卿之选，以翼京师；八屯之权，实资宿卫。历纪授任，一心靡渝。今上祇嗣鸿图，益宣朝寄，总千牛之士以为心膂，假五教之秩以崇班列。会侍中燕王以帝子之重，兼镇两藩，详求命卿，以事大国，俾公提步卒屯宣城，凡甲兵壁垒之事，皆听于公。夙夜惟勤，燥湿生疾，春秋六十一，保大九年十月七日卒于宣州公署。上省奏伤悼，为之罢朝，送终之礼，有以加等。即以其年十二月二十七日，葬于江宁府县里，礼也。夫人王氏，淮南裨将唐之长女也。先公负游侠之气，有征讨之功，勇冠三军，力制奔虎。夫人丽桃李之质，袭兰薰之芳，妇礼聿修，遗训无坠。君子以孝慈率教，夫人以严正克家，闺门之理，实有内助。以保大八年五月一日先公而逝，今始祔焉。子全厚、全赡、全节、全义、全海，皆有父风，苗氏为不朽也。铉本自世亲，早为姻族。叹侯封于李广，发哀词于杜笃。刻翠琰于荒千，拟高陵于深谷。其铭曰：才之俊兮将之雄，位之侯兮寿未中。天难谌兮人云亡，川既逝兮岁将穷。素车兮丹旐，白艸兮青松。悲雄心与壮气，渐荆棘兮蒙笼。《徐公文集》卷一六。又见《全唐文》卷八八六。</t>
+          <t>公諱文蔚，字君章。其先濟陽考城人也。昔高陽恢若水之靈，光有萬國；伯益獲箕山之護，克成夏功。故其子孫，延祚丕顯，茅土錫胤，圭組流光。在漢者爲孝子，在宋者爲忠宰，在梁者爲烈將，在陳者爲詞臣。長城既封，淮水亦絶，辭周粟而遠騖，避嬴亂而深藏，徙籍建安，世爲大姓。至于我王考毗、考秦，皆以隱德清操，垂爲門風。惟公嗣奕葉之賢，有生知之異，幼挺奇表，夙韜殊量。殫儒墨之秘奧，窮文史之菁英。閭里歸仁，宗黨稱孝。于時天下未一，遐方不寧，公鄙尺鷃之爲，從黃鵠之舉，類延州之觀樂，同太史之探書，升名俊造，從事河洛。衰俗難佐，天壤不支。我烈祖孝高皇帝，王業始于江東，仁風被于四裔，公杖策高蹈，款關來儀。府朝肅以生風，臺閣藹其增氣。署宣州觀察巡官，試秘書郎，遷水部員外郎，賜緋魚袋。王國初建，改比部員外郎，知制誥。于時天人協應，獄訟攸歸，舜、禹相與言，游、夏不能措，潤色之任，我則無慚。既受禪，遷主客郎中，知制誥如故。俄而真拜，仍賜金紫。今上嗣位，大禮聿修，徙公爲給事中，判太常卿事。時同軌胥會，有司失職，公與司門郎中蕭君儼、博士韓君熙載，協力建儀，周行翕然。由是祖功宗德之位定，大行昭名之義允，功署高廟，與天無窮。明年，拜御史中丞，矯枉持平，無所顧憚，坐廷劾宰相，其言深切，貶江州司士參軍。初，國朝自王義方之後〔一〕，曠數百年，憲署之間，舉無廢職〔二〕，然未有危言激論如此之彰灼者也。故權右振竦，朝野喧騰，傳寫彈文，爲之紙貴。人心既爾，天鑑亦迴，前所劾者，或免或黜，公就加江州營田副使。頃之，徵爲衛尉卿。俄拜右諫議大夫，充翰林學士，權知貢舉。出納密命，樞機靡失，登進造士，衡鏡無私，聳禁署之清風，著春官之故事。薦賢之賞，行及于台司；曳杖之期，奄先于朝露。春秋五十有二，保大十年八月二日卒于京師官舍。皇上痛惜，爲之廢朝，送死卹孤，一從公賜。有司考行，易名曰簡。即以其年九月十三日，葬于某縣某里之原，禮也。長子翥，秘書省正字，次子鶱，皆早卒。今以從子翹爲嗣。嗚呼哀哉!公心平氣和，貌古神正。雅好玄理，有方外之期；尤善詞賦，得《國風》之體。去華簡禮，不以位望驕人；憐才誘善，不以威名傲物。操履堅正，靡得動搖；襟懷坦夷，初無蒂介。謫居江楚，恬然自足。孜孜色養，烝烝孝心。嘗爲詩云：‘屈平若遇高堂在，應不懷沙獨葬魚。’此其心也。江州節度使賈公崇，以武立功，以剛肅物，事公如師傅，親公如兄弟。時皆服公之重名，而賢賈之樂善也。既歸京，寓居公廨，無以家爲。二子繼亡，一慟而已。齊死生于夢覺，遺寵辱于錙銖，古之達者，何以過此。嗚呼!凡我僚舊，均哀共戚。入黔婁之門閫，覽伯喈之經籍。睇落日以流慟，愬秋風而沾臆。企景行于高山，勒哀詞于樂石。其詞曰：高陽之裔，伯益之孫。展矣君子，載大其門。爰翔爰集，樂我樹檀。彯纓幕府，振藻西垣。禮儀卒獲，風憲攸端。道行在時，業隆自我。英英若人，見義必果。直指烈烈，宮鄰瑣瑣。死生以之，何適不可?允矣天鑑，明哉主恩。乃還宣室，乃入脩門。從容禁署，密勿王言。得才爲盛，知人則難。求尸宗伯，載善其官。人必有終，古無不死。嗟嗟若人，風流永矣。徐庶有母，鄧攸無子。闕里諸生，荊州故吏。謂之何哉?啜其泣矣。秋風落木，逝水成川。昨朝飛蓋，今日荒阡。一丘殘照，萬古愁煙。素車自返，寶劍高懸。高才兮直道，共盡兮何言!《徐公文集》卷一五。又見《全唐文》卷八八五。〔一〕方：原脫，據徐校、李校補。〔二〕間舉：原作‘舉間’，據《全唐文》、李刊本乙。</t>
         </is>
       </c>
       <c r="L5" t="n">
@@ -732,35 +732,31 @@
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>2</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>邻;唐</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
         <v>0</v>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
-          <t>10;南唐</t>
+          <t>6;唐</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4967079</t>
+          <t>4967008</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>403940</v>
+        <v>394761</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>方讷</t>
+          <t>周廷構</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -780,7 +776,7 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>公讳讷，字希仁。其先河南人也，后世从官，徙籍新安，支派繁衍，遂为郡之著姓。迨公数世，皆以儒雅退让，播为门风。曾祖颙，登州文登县令。祖亮，左武卫兵曹参军。考縠，荣王府司马。母聂氏，追封河南县太君，问政先生师道之长女也。公承积善之庆，负夙成之智，砥节励行，好学能文，时然后言，非礼勿动，乡曲之党，翕然称之。太师陶公，来守新安，抚纳人士，署为郡吏，委以典签，恪恭详敏，甚称所职。历事累政，其志如初。烈祖肇基王业，元宗实综军政，管记之任，勤择其人，闻公之名，召致幕府。王国初建，署宁国军节度馆驿巡官，掌都统表奏。皇室再造，庆赏遂行，擢拜虞部员外郎，掌元帅表奏。数岁，以皇孙就傅，命公侍读。讲道赞德，励裨益之诚；端己直躬，尽表微之节。俄迁水部郎中。明年，皇孙封南昌王、东都留守，以公为留守判官，迁主客郎中，参赞政务，事无违者。改司农少卿，依前充职。明年，王移任宣、润二州大都督，复以公为浙西营田副使，通判军府。六载匪懈，庶职交修，懋官之赏，诏命叠委。累迁至金紫光禄大夫、检校司徒，封河南县男。俄拜泰州刺史，充本州屯田监院使。正身而令，悉心为理，公无遗利，民自从风。属强敌深侵，东京失守，而州兵尽出，人心大摇。于是士庶老幼，尽室南渡。公自归阙下，坐是除名。数年，除歙州团练判官，上曰：‘战争之际，吾岂以武勇责书生哉〔一〕!军法不得不尔。’即召拜太子右谕德。今上嗣位，迁少府监。丙寅岁正月十六日，卒于京师美仁坊官舍，享年七十七。上为之废朝一日，赐谥曰定。以其年某月日葬于某所，礼也。前夫人谢氏早亡，继室施氏封沛县君。长子前，宣州宁国县主簿；次子志，饶州文学。公以名教为乐，以矩矱自任，行必中立，居无惰容，[748]CE7C[/748]绅之间，推为纯行。公之外祖，得道之士，故公颇以朝礼修养为务，鸡鸣而起，孜孜不倦。年俯悼耄，体常康强，及属纩之晨，无伏枕之疾，斯亦力行之报也。铉也不佞，早辱交契。昔先君从事黟、歙，公适仕本部。及公策名郎署，铉亦忝官联。既熟其素履，愿垂于不朽，附于史氏，以永令猷。其铭曰：圣人四教：文行忠信。惟公似之，光有令问。秉笔赞画，登朝典郡。宠至若惊，道丧无闷。年俯中寿，官参列卿。归全委顺，终吉永贞。宰树长在，高台自倾。用刊圆石，閟此佳城。《徐公文集》卷一五。又见《全唐文》卷八八五。〔一〕责：原作‘贵’，据《全唐文》、黄校本、李刊本改。</t>
+          <t>君諱廷構，字正材，洛陽人也。岐山至德，綿瓜瓞者萬邦；洛宅舊都，守枌榆者百世。簪組相繼，譜諜存焉。曾祖侃，太常博士。祖潛，深州樂壽縣令。避亂南徙，因家廣陵。考延禧，明經擢第。有吳之霸，受辟爲淮南巡官，累官至戶部郎中，與殷文公、游貞公同掌文翰。無祿早世，故大位不躋。君即戶部第四子也。幼而岐嶷，長而篤厚，躬行孝悌，餘力學文。以蔭釋褐，補弘文館校書，試吏爲池州司戶參軍，改宣州寧國縣尉。烈祖在藩，乃睠舊族，聞君修謹，復有吏能，因表爲黃州長史，寵以朱紱，置之府朝。及受禪，遷通事舍人。鴻業肇興，王澤遐布，贊導之任，實寄司聰，護戎修聘，觀風按獄，受命而出，動罔不臧。歷事兩朝，任遇彌厚，賞賜既數，階勳屢遷，而通事之任如故，蓋惜其能也。保大七年，轉將作少監，判四方館事。浩穰之地，尹正爲難，復以本官判江寧府事。其間監諸侯之典者十，通四方之命者三，攝州府之政者六，按枉撓之獄者四。或敷惠于新附之俗，或投身于危亂之地，本于忠而後動，忘其生而後存。元宗嘉之，以爲客省使。今上嗣位，深惟舊勞，特加金紫光祿大夫、台州刺史。常御壽昌殿視事，中外之人，咸得引見，又以君爲壽昌殿承宣。出爲忠義軍監軍、泉南等州宣諭使。還，遷筠州刺史、本州團練，仍使充客省使。君以備嘗艱危，復逼遲暮，懇辭繁劇，恩旨不從。丙寅歲十月二十二日，終于京師某里之官舍，春秋六十有六。詔廢朝一日，賜諡曰某。明年正月日葬于某所，禮也。夫人天水縣君姜氏，輔佐之勤，率由婦禮，訓誨諸子，備有義方。子大理評事崇儉，太常寺奉禮郎崇素，及崇順、崇信等，皆儒謹，且不墜其先。鉉家世通舊，嘗接姻婭，淡成之分，終始不渝。何以寘懷，是用刊德。其銘曰：猗嗟周君，世濟其名。展如之人，克嗣厥聲。受任幹蠱，臨難忘身。居中處約，全和保真。與物皆化，萬古同塵。松楸勿伐，蘭菊惟新。刊石表墓，于嗟善人!《徐公文集》卷一五。又見《全唐文》卷八八五。</t>
         </is>
       </c>
       <c r="L6" t="n">
@@ -804,53 +800,41 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4967108</t>
+          <t>4967079</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>92561</v>
+        <v>403940</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>乔匡舜</t>
+          <t>方訥</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>亚元;贞</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>高邮</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>士有放怀夷旷，介然中立，外物无累于心，没齿不违于道，吾友乔公尝从事于斯矣。公讳匡舜，字亚元，广陵高邮人也。曾祖谭、祖泰，皆不仕。考鸿渐，本县尉。家世清操，州闾称之，故其子孙必有兴者。公少好学，善属文，弱冠游京都，词藻典丽，容止都雅。烈祖辅政，见而器之，补秘书省正字。丞相宋楚公，初获进用，位望日崇，闻公之名，辟置门下，每为文赋诗咏，辄加称赏。由是名誉日洽，而卿士大夫皆前席待之。累迁大理评事、司直、监察御史、屯田员外郎，从宋公出藩，为江西、浙西掌书记。府公告老归九华山，公乃升朝，为驾部员外郎。未几，守本官知制诰，就迁祠部郎中、中书舍人。典掌枢机，周慎静默，凡十余年。值边境俶扰，师出无功，诏旨亲征，中外忧惧，公上疏极谏，坐沮挠军势，黜居临川。顷之，宋公获谴，又以故吏为累，由是累年沈废。今上即位，征为水部员外郎，改司农少卿，判太常寺，转殿中监，修国史，拜给事中，权知贡举，又兼献纳使，迁刑部侍郎。公自征还，数年间联历清望，盖旧齿直道，上简圣心。至是，以老病不堪朝谒闻，上知其家贫，诏以二卿之秩养疾。壬申岁九月二十有三日，卒于京师滨江里官舍，享年七十有五，遗命以《周易》、《孝经》置棺中。太常考行，易名曰贞。即以其年冬十月二十有三日，葬于江宁县某所，礼也。夫人太原县君郭氏，代公玄孙、晋陵令喻之女也。余庆所备，门风甚高，妇德母仪，闻于宗族。一子僧孺，秘书省正字，早卒。孙谞，亦为正字。公之为人，宽简真率，常以诗酒自适，不以势利萦心，毁誉谗慝之词闻之晏如也。从事楚公府殆二十年，凡为府公见知者皆诡谲倾侧，公独淡然无营，守正不谄〔一〕，故但以文义知赏，末尝任用。烈祖下诏公卿，举可以亲民者。楚公所荐非其人，烈祖甚不悦，谓给事中常公梦锡曰：‘吾望其荐匡舜也。’常公及中书侍郎韩公熙载，嫉楚公如雠，而与公善，尝相谓曰：‘宋公误识亚元，正可怪也。’公之历任，奉法循理，似不能言者，及其临危击节，抗词忤旨，侃侃然有古人之风。黜官夺禄，甘贫守约，凡五年不形于言色，恂恂然道家之流也。故能享老寿，保康宁，归全委顺，斯可贵矣。公临终数日，舍弟往候之，怡然言曰：‘吾往矣，君兄弟可各为一诗哭我。’翌日，复告门生曰：‘吾已得徐君兄弟许我诗，余无事矣。’其忘怀死生也如此。呜呼!絮酒之礼，已隔平生；挂剑之信，永畀穹壤。故以二章为志，閟于九原。所撰集七十余卷，编纪之任，属于门人，此不备书也。其诗云：举世重文雅，夫君更质真。曾嗟混鸡鹤，终自异淄磷。词赋离骚客，封章谏诤臣。襟怀道家侣，标格古时人。逸老诚云福，遗形未免贫。求文空得艸，埋玉遂为尘。静想忘年契，冥思接武晨。连宵洽杯酒，分日掌丝纶。蠹简书陈事，遗孤托世亲。前贤同此叹，非我独沾巾。锴诗云：诸公长者郑当时，事事无心性坦夷。但是登临皆有作，未尝相见不伸眉。生前适意无过酒，身后遗言只要诗。三日笑谈成理命，一篇投吊尚应知。《徐公文集》卷一六。又见《全唐文》卷八八六。〔一〕正：原作‘政’，据《全唐文》、黄校本改。</t>
+          <t>公諱訥，字希仁。其先河南人也，後世從官，徙籍新安，支派繁衍，遂爲郡之著姓。迨公數世，皆以儒雅退讓，播爲門風。曾祖顒，登州文登縣令。祖亮，左武衛兵曹參軍。考縠，榮王府司馬。母聶氏，追封河南縣太君，問政先生師道之長女也。公承積善之慶，負夙成之智，砥節勵行，好學能文，時然後言，非禮勿動，鄉曲之黨，翕然稱之。太師陶公，來守新安，撫納人士，署爲郡吏，委以典籤，恪恭詳敏，甚稱所職。歷事累政，其志如初。烈祖肇基王業，元宗實綜軍政，管記之任，勤擇其人，聞公之名，召致幕府。王國初建，署寧國軍節度館驛巡官，掌都統表奏。皇室再造，慶賞遂行，擢拜虞部員外郎，掌元帥表奏。數歲，以皇孫就傅，命公侍讀。講道贊德，勵裨益之誠；端己直躬，盡表微之節。俄遷水部郎中。明年，皇孫封南昌王、東都留守，以公爲留守判官，遷主客郎中，參贊政務，事無違者。改司農少卿，依前充職。明年，王移任宣、潤二州大都督，復以公爲浙西營田副使，通判軍府。六載匪懈，庶職交修，懋官之賞，詔命疊委。累遷至金紫光祿大夫、檢校司徒，封河南縣男。俄拜泰州刺史，充本州屯田監院使。正身而令，悉心爲理，公無遺利，民自從風。屬強敵深侵，東京失守，而州兵盡出，人心大搖。于是士庶老幼，盡室南渡。公自歸闕下，坐是除名。數年，除歙州團練判官，上曰：‘戰爭之際，吾豈以武勇責書生哉〔一〕!軍法不得不爾。’即召拜太子右諭德。今上嗣位，遷少府監。丙寅歲正月十六日，卒于京師美仁坊官舍，享年七十七。上爲之廢朝一日，賜謚曰定。以其年某月日葬于某所，禮也。前夫人謝氏早亡，繼室施氏封沛縣君。長子前，宣州寧國縣主簿；次子志，饒州文學。公以名教爲樂，以矩矱自任，行必中立，居無惰容，[748]CE7C[/748]紳之間，推爲純行。公之外祖，得道之士，故公頗以朝禮修養爲務，鷄鳴而起，孜孜不倦。年俯悼耄，體常康強，及屬纊之晨，無伏枕之疾，斯亦力行之報也。鉉也不佞，早辱交契。昔先君從事黟、歙，公適仕本部。及公策名郎署，鉉亦忝官聯。既熟其素履，願垂于不朽，附于史氏，以永令猷。其銘曰：聖人四教：文行忠信。惟公似之，光有令問。秉筆贊畫，登朝典郡。寵至若驚，道喪無悶。年俯中壽，官參列卿。歸全委順，終吉永貞。宰樹長在，高臺自傾。用刊圓石，閟此佳城。《徐公文集》卷一五。又見《全唐文》卷八八五。〔一〕責：原作‘貴’，據《全唐文》、黃校本、李刊本改。</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>13</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>大理评事;祠部郎中;殿中监;给事中;驾部员外郎;秘书省正字;司农少卿;水部员外郎;屯田员外郎;刑部侍郎;修国史;知制诰;中书舍人</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>0</v>
       </c>
@@ -868,49 +852,57 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4967120</t>
+          <t>4967108</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27034</v>
+        <v>92561</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>赵宣辅</t>
+          <t>喬匡舜</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>亞元;貞</t>
+        </is>
+      </c>
       <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>高郵</t>
+        </is>
+      </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>君讳宣辅，字仲申。其先天水人也，累世从宦，不常厥居。曾祖全真，工部员外郎、滕州刺史。祖倚，太子校书。考台，歙州海宁令。君即海宁府君第三子也，生于广陵，长于江左。幼而俊敏，博综群书，尤善名法之学〔一〕。烈祖辅政，方申明纪律，君以是中选，释褐补江都府文学，直刑部。明年，改信州司法参军，察狱详刑，号为详练。久之，召赴阙，以本官权参元帅府法曹事。逾年，改大理评事。元宗嗣服之初，精心庶狱，权要举不附己者，因中伤之，君坐黜为饶州司士参军。明年，王师伐闽，护军查公表君才可烦，使以本官判军司事。时顿兵深入，自冬涉秋，经束马悬车之涂，督飞刍挽粟之役，事集师克，君有力焉。师还，加朝散大夫，行常州义兴令，推诚率下，民用协和。丁忧去职，复为江州录事参军。时连帅议浚湓浦，以屯舟师，诏从之。君以无益戎备而劳民力，乃指陈利害，抗疏极论。上甚嘉之，即命止役。由是迁大理司直，通判蕲州军州事。明年，迁检校水部员外郎，充建州观察推官，通判军府事。会越人窥边，使间诱建民，将以为乱。君廉得其实，尽案诛之。优诏褒美，赐衣一袭，迁检校屯田员外郎。三年，征拜守水部员外郎，判度支。时师旅荐兴，军食不给，命君为沿江催运使，轺傅所至，转输如流。朝议以姑熟居畿甸之间，实供亿之始，徙君为当涂令。逾月，复征为主客员外郎，判大理寺，赐紫金鱼袋。始君以理官得罪，至是上知其无私，故复任焉。守官循理，挺然中立，转工部员外郎，仍判寺事。今上嗣位，上疏论时政，以为刺史县令，亲民之先，而考绩抡材，未尽其理。上深然之，迁朝议大夫、户部员外，充宣、歙、常、润等道安抚使。以刺举无避，为权臣所排，宸鉴昭明，故得无咎。使还，以本官判兵部事。庐陵群盗充斥，州兵不能制，上忧之，亟命君为奉化军节度判官，判吉州事，转主客郎中，擒奸摘伏，克举其职。其年秋九月七日遇暴疾，翌日终于郡之官舍，享年六十有一。明年春二月，归葬江宁府某所，礼也。夫人查氏，吉王府长史昌之女、工部尚书文徽之妹。婉嫟之德，闺房之秀，内助著美，士林所推。子七人：长曰钧，袁州新喻尉；次曰错，枢密院承旨；次曰钟，举进士；次曰铨，前国子监三《礼》；次曰[CFont]NFCE5[/CFont]、钺、鐭，皆国子监生。女一人，适秘书省正字周希定。君有孝悌之性，闻于宗族；惇然诺之信，称于友朋。守己有常，事君不谄。位未达而知足，禄虽优而弥贫。其当官持事也，必尽己所长，不为利回，不为威惕，故屡失大臣意，然好直之士亦以此多之。铉久尘近职，熟君操行，直笔耸善，以告后人，故铭其墓曰：英英赵君，松茂兰薰。应用以法，饰身以文。道直词正，心平气纯。如何不淑，今也为尘。金陵仙乡，古多名人。归骨于是，与善为邻。泉台不晓，垄树空春。勒铭挂剑，慷慨沾巾。《徐公文集》卷一五。又见《全唐文》卷八八六。〔一〕名：原作‘身’，据《全唐文》、徐校、李校、四库本改。</t>
+          <t>士有放懷夷曠，介然中立，外物無累于心，没齒不違于道，吾友喬公嘗從事于斯矣。公諱匡舜，字亞元，廣陵高郵人也。曾祖譚、祖泰，皆不仕。考鴻漸，本縣尉。家世清操，州閭稱之，故其子孫必有興者。公少好學，善屬文，弱冠游京都，詞藻典麗，容止都雅。烈祖輔政，見而器之，補秘書省正字。丞相宋楚公，初獲進用，位望日崇，聞公之名，辟置門下，每爲文賦詩詠，輒加稱賞。由是名譽日洽，而卿士大夫皆前席待之。累遷大理評事、司直、監察御史、屯田員外郎，從宋公出藩，爲江西、浙西掌書記。府公告老歸九華山，公乃升朝，爲駕部員外郎。未幾，守本官知制誥，就遷祠部郎中、中書舍人。典掌樞機，周慎靜默，凡十餘年。值邊境俶擾，師出無功，詔旨親征，中外憂懼，公上疏極諫，坐沮撓軍勢，黜居臨川。頃之，宋公獲譴，又以故吏爲累，由是累年沉廢。今上即位，徵爲水部員外郎，改司農少卿，判太常寺，轉殿中監，修國史，拜給事中，權知貢舉，又兼獻納使，遷刑部侍郎。公自徵還，數年間聯歷清望，蓋舊齒直道，上簡聖心。至是，以老病不堪朝謁聞，上知其家貧，詔以二卿之秩養疾。壬申歲九月二十有三日，卒于京師濱江里官舍，享年七十有五，遺命以《周易》、《孝經》置棺中。太常考行，易名曰貞。即以其年冬十月二十有三日，葬于江寧縣某所，禮也。夫人太原縣君郭氏，代公玄孫、晉陵令喻之女也。餘慶所備，門風甚高，婦德母儀，聞于宗族。一子僧孺，秘書省正字，早卒。孫諝，亦爲正字。公之爲人，寬簡真率，常以詩酒自適，不以勢利縈心，毀譽讒慝之詞聞之晏如也。從事楚公府殆二十年，凡爲府公見知者皆詭譎傾側，公獨淡然無營，守正不諂〔一〕，故但以文義知賞，末嘗任用。烈祖下詔公卿，舉可以親民者。楚公所薦非其人，烈祖甚不悅，謂給事中常公夢錫曰：‘吾望其薦匡舜也。’常公及中書侍郎韓公熙載，嫉楚公如讎，而與公善，嘗相謂曰：‘宋公誤識亞元，正可怪也。’公之歷任，奉法循理，似不能言者，及其臨危擊節，抗詞忤旨，侃侃然有古人之風。黜官奪祿，甘貧守約，凡五年不形于言色，恂恂然道家之流也。故能享老壽，保康寧，歸全委順，斯可貴矣。公臨終數日，舍弟往候之，怡然言曰：‘吾往矣，君兄弟可各爲一詩哭我。’翌日，復告門生曰：‘吾已得徐君兄弟許我詩，餘無事矣。’其忘懷死生也如此。嗚呼!絮酒之禮，已隔平生；掛劍之信，永畀穹壤。故以二章爲誌，閟于九原。所撰集七十餘卷，編紀之任，屬于門人，此不備書也。其詩云：舉世重文雅，夫君更質真。曾嗟混雞鶴，終自異淄磷。詞賦離騷客，封章諫諍臣。襟懷道家侶，標格古時人。逸老誠云福，遺形未免貧。求文空得草，埋玉遂爲塵。靜想忘年契，冥思接武晨。連宵洽杯酒，分日掌絲綸。蠹簡書陳事，遺孤託世親。前賢同此歎，非我獨霑巾。鍇詩云：諸公長者鄭當時，事事無心性坦夷。但是登臨皆有作，未嘗相見不伸眉。生前適意無過酒，身後遺言只要詩。三日笑談成理命，一篇投弔尚應知。《徐公文集》卷一六。又見《全唐文》卷八八六。〔一〕正：原作‘政’，據《全唐文》、黃校本改。</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>大理評事;祠部郎中;殿中監;給事中;駕部員外郎;秘書省正字;司農少卿;水部員外郎;屯田員外郎;刑部侍郎;修國史;知制誥;中書舍人</t>
+        </is>
+      </c>
       <c r="N8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>台</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
         <v>0</v>
       </c>
@@ -924,39 +916,35 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4967201</t>
+          <t>4967120</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>119793</v>
+        <v>27034</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>樊潜</t>
+          <t>趙宣輔</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>贵池</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>公讳潜，字仲明，京兆万年人也。昔者虞仲垂孙谋之庆，肇启我封；山甫昭补职之勤，实大吾族。或则游圣门而称达者，或则冠仙籍而号真人〔一〕。丰沛功臣，经营于大业；南阳外戚，佐佑于中兴。傅祀百世〔二〕，流光万国。而我之占籍，世茂西京，樊川之居，抗衡韦、杜。曾祖澄，以七世同爨，孝德升闻，大中制恩，特加旌表，峨峨石阙，至今存焉。祖偁，濮州司户参军。考谕，光化中补池州至德令，时天下已乱，因家池阳，终润州金坛令。公中和禀粹，形器夙成。好学之勤，本由天赋；至孝之性，不坠家声。始及弱冠，并违怙恃。绝浆泣血，哀感州闾。负土成坟，终丧庐墓。言子道者，以为美谈。于时唐祚沦胥，宗室称制，江淮之地，不失旧章。公以射策高等，补润州丹阳尉，试吏之课，书考为优。庐陵之民，古称多讼，加以亩籍违制，乱狱滋丰。守臣上言，求拯其弊。有命择堪其事者，闻公之能，因而命之。公既至，乃相五土之沃瘠，察夫家之众寡，采古之制，酌今之宜，创为新规，众皆悦服。而复出械系之者〔三〕，穷两造之辞〔四〕，雪当死者数十人。使还议赏，增秩进等，迁寿州寿春县主簿。既而庐陵之政日理，南楚之人耸观。久之，以公为光州光山县令，加大理评事，犹以前效也。于时南北分裂，县临敌境，有争桑之女，多探丸之吏〔五〕，比闾之众，罕尝宁居。公于是纠集义勇，分守要害，推以恩信，济之强明，三载之中，一邑用乂。迁池州石埭令。县有大姓，侵挠细民，岁比不登，俗乃重困。公绳之以法，董之以威，豪右震憡，相与逃匿。于是启请出官粟以赈乏，绝省力役，以济农功。慈抚仁薰，视之如子，岁丰俗阜，政用大成。就加大理司直，旌能政也。秩满，迁鄂州汉阳令。未几遇疾，壬子岁某月日，终于县之正寝，享年五十有七。以丙辰岁某月日葬于池州贵池县永泰乡保静里之原，礼也。夫人王氏，鸿胪卿滔之女。轩冕之族，闺房之秀，室家垂训，惠问风行。长子若讷，不事王侯，自全高尚。次子知古，才艺毕给，际会昌朝，践历台省，交修繁剧，今为右谏议大夫、河北转运使，扬名之业方茂，显亲之数遂优。公累赠秘书丞、户部员外郎、卫尉少卿。夫人封琅邪县太君。惟公生而岐嶷，长而学问，穷九经之奥旨，综百氏之微言。率是古道，施于为政，行之以直，守之以廉，事亲以孝，饰躬以礼。士元之器，命屈于生前；臧孙之忠，庆贻于身后。君恩饰壤，世禄傅家，咸京之旧表未堙，秋浦之丰碑复立，俗有遗爱，吾无愧辞。其铭曰：南山崇崇，樊川溶溶。剪商之烈，补衮之功。百代之后，流光不穷。爰有孝德，克生我公。猗欤我公，显允君子。投此利刃，行于百里。有惠于民，何必贵仕；垂庆于后，何必在己!庆霄之泽，自叶流根。歾垂中佃，生驾鱼轩。二子殊志，具大吾门。僾僾愚谷，英英谏垣。九峰之下，贵池之口。覆斧马鬣，金鸡玉狗。民即桐乡，碑如岘首。江水长流，令名同久。《徐公文集》卷二七。〔一〕仙：原作‘先’，据徐校、李刊本改。〔二〕祀：原作‘杞’，据徐校、黄校本、本刊本改。〔三〕‘者’字疑误。〔四〕辞：原作‘乱’，据黄校本、李刊本改。〔五〕丸：原作‘九’，据徐校、黄校本、李刊本改。</t>
+          <t>君諱宣輔，字仲申。其先天水人也，累世從宦，不常厥居。曾祖全真，工部員外郎、滕州刺史。祖倚，太子校書。考臺，歙州海寧令。君即海寧府君第三子也，生于廣陵，長于江左。幼而俊敏，博綜羣書，尤善名法之學〔一〕。烈祖輔政，方申明紀律，君以是中選，釋褐補江都府文學，直刑部。明年，改信州司法參軍，察獄詳刑，號爲詳練。久之，召赴闕，以本官權參元帥府法曹事。踰年，改大理評事。元宗嗣服之初，精心庶獄，權要舉不附己者，因中傷之，君坐黜爲饒州司士參軍。明年，王師伐閩，護軍查公表君才可煩，使以本官判軍司事。時頓兵深入，自冬涉秋，經束馬懸車之塗，督飛芻輓粟之役，事集師尅，君有力焉。師還，加朝散大夫，行常州義興令，推誠率下，民用協和。丁憂去職，復爲江州録事參軍。時連帥議浚湓浦，以屯舟師，詔從之。君以無益戎備而勞民力，乃指陳利害，抗疏極論。上甚嘉之，即命止役。由是遷大理司直，通判蘄州軍州事。明年，遷檢校水部員外郎，充建州觀察推官，通判軍府事。會越人闚邊，使間誘建民，將以爲亂。君廉得其實，盡案誅之。優詔褒美，賜衣一襲，遷檢校屯田員外郎。三年，徵拜守水部員外郎，判度支。時師旅荐興，軍食不給，命君爲沿江催運使，軺傳所至，轉輸如流。朝議以姑熟居畿甸之間，實供億之始，徙君爲當塗令。踰月，復徵爲主客員外郎，判大理寺，賜紫金魚袋。始君以理官得罪，至是上知其無私，故復任焉。守官循理，挺然中立，轉工部員外郎，仍判寺事。今上嗣位，上疏論時政，以爲刺史縣令，親民之先，而考績掄材，未盡其理。上深然之，遷朝議大夫、戶部員外，充宣、歙、常、潤等道安撫使。以刺舉無避，爲權臣所排，宸鑑昭明，故得無咎。使還，以本官判兵部事。廬陵羣盗充斥，州兵不能制，上憂之，亟命君爲奉化軍節度判官，判吉州事，轉主客郎中，擒奸摘伏，克舉其職。其年秋九月七日遇暴疾，翌日終于郡之官舍，享年六十有一。明年春二月，歸葬江寧府某所，禮也。夫人查氏，吉王府長史昌之女、工部尚書文徽之妹。婉嬺之德，閨房之秀，內助著美，士林所推。子七人：長曰鈞，袁州新喻尉；次曰錯，樞密院承旨；次曰鍾，舉進士；次曰銓，前國子監三《禮》；次曰[CFont]NFCE5[/CFont]、鉞、鐭，皆國子監生。女一人，適秘書省正字周希定。君有孝悌之性，聞于宗族；敦然諾之信，稱于友朋。守己有常，事君不諂。位未達而知足，祿雖優而彌貧。其當官持事也，必盡己所長，不爲利回，不爲威惕，故屢失大臣意，然好直之士亦以此多之。鉉久塵近職，熟君操行，直筆聳善，以告後人，故銘其墓曰：英英趙君，松茂蘭薰。應用以法，飾身以文。道直詞正，心平氣純。如何不淑，今也爲塵。金陵仙鄉，古多名人。歸骨于是，與善爲鄰。泉臺不曉，壟樹空春。勒銘掛劍，慷慨霑巾。《徐公文集》卷一五。又見《全唐文》卷八八六。〔一〕名：原作‘身’，據《全唐文》、徐校、李校、四庫本改。</t>
         </is>
       </c>
       <c r="L9" t="n">
@@ -964,35 +952,31 @@
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>知古</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
         <v>0</v>
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
-          <t>15;宋</t>
+          <t>10;南唐</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4967204</t>
+          <t>4967120</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>36351</v>
+        <v>449301</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>王煜</t>
+          <t>趙宣輔</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1012,7 +996,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>盛德百世，善继者所以主其祀；圣人无外，善守者不能固其存。盖运历之所推，亦古今之一贯。其有享蕃锡之宠，保克终之美，殊恩饰壤，懿范流光，傅之金石，斯不诬矣。王讳煜，字重光，陇西人也。昔庭坚赞九德，伯阳恢至道。皇天眷祐，锡祚于唐，祖文宗武，世有显德。载祀三百，龟玉沦胥，宗子维城，蕃衍万国。江淮之地，独奉长安，故我显祖，用膺推戴。淳耀之烈，载光旧吴。二世承基，克广其业。皇宋将启，玄贶冥符。有周开先，太祖历试。威德所及，寰宇将同。故我旧邦，祇畏天命，贬大号以禀朔，献地图而请吏。故得义动元后，风行域中，恩礼有加，绥怀不世。鲁用天王之礼，自越常钧；酅存纪侯之国，曾何足贵?王以世嫡嗣服，以古道驭民，钦若彝伦，率循先志。奉蒸尝、恭色养必以孝，宾大臣、事耇老必以礼，居处服御必以节，言动施舍必以时。至于荷全济之恩，谨藩国之度，勤修九贡，府无虚月，祇奉百役，知无不为。十五年间，天眷弥渥。然而果于自信，怠于周防，西邻起衅，南箕构祸。投杼致慈亲之惑，乞火无里妇之辞。始劳因垒之师，终后涂山之会。太祖至仁之举，大赉为怀，录勤王之前效，恢焚谤之广度，位以上将，爵为通侯，待遇如初，宠锡斯厚。今上宣猷大麓，敷惠万方，每侍论思，常存开释。及飞天在运，丽泽推恩，擢进上公之封，仍加掌武之秩。侍从亲礼，勉谕优容。方将度越等彝，登崇名数。呜呼!阅川无舍，景命不融，太平兴国三年秋七月八日遘疾，薨于京师里第〔一〕，享年四十有二。皇上抚几兴悼，投瓜轸悲，痛生之不逮，俾歾而加饰，特诏辍朝三日，赠太师，追封吴王，命中使莅葬，凡丧祭所须，皆从官给。即其年冬十月日，葬于河南府某县某乡某里，礼也。夫人郑国夫人周氏，勋旧之族，是生邦媛，肃雍之美，流咏国风，才实女师，言成梱则。子左千牛卫大将军某〔二〕，襟神俊茂，识度淹通，孝悌自表于天资，才略靡由于师训，日出之学，未易可量。惟王天骨秀异，神气清粹。言动有则，容止可观。精究六经，旁综百氏。常以为周、孔之道不可暂离，经国化民，发号施令，造次于是，终始不渝。酷好文辞，多所述作。一游一豫，必颂宣尼〔三〕；载笑载言，不忘经义。洞晓音律，精别雅郑。穷先王制作之意，审风俗淳薄之原，为文论之，以续《乐记》。所著文集三十卷，杂说百篇，味其文知其道矣。至于弧矢之善，笔札之工，天纵多能，必造精绝。本以恻隐之性，仍好竺干之教，艸木不杀，禽鱼咸遂。赏人之善，常若不及；掩人之过，惟恐其闻。以至法不胜奸，威不克爱，以厌兵之俗，当用武之世。孔明罕应变之略，不成近功；偃王躬仁义之行，终于亡国。道有所在，复何愧欤?呜呼哀哉!二室南峙，三川东注。瞻上阳之宫阙，望北邙之灵树。旁寂寂兮迥野，下冥冥兮长暮。寄不朽于金石，庶有傅于竹素。其铭曰：天鉴九德，锡我唐祚。绵绵瓜瓞，茫茫商土。裔孙有庆，旧物重睹。开国承家，疆吴跨楚。丧乱孔棘，我恤畴依。圣人既作，我知所归。终日靡俟，先天不违。惟藩惟辅，永言固之。道或污隆，时有险易。蝇止于棘，虎游于市。明明大君，宽仁以济。嘉尔前哲，释兹后至。亦觏亦见，乃侯乃公。沐浴玄泽，徊翔景风。如松之茂，如山之崇。奈何不淑，运极化穷。旧国疏封，新千启室。人谂之谋，卜云其吉。龙章骥德，兰言玉质。邈尔何往?此焉终毕。俨青盖兮裶裶，驱素虬兮迟迟。即隧路兮徒返，望君门兮永辞。庶九原之可作，与缑岭兮相稘。垂斯文于亿载，将乐石兮无亏。《徐公文集》卷二九。又见《皇朝文鉴》卷一三九。〔一〕京师里第：原作‘京师里之第’。徐校、李校云：‘师’下疑有脱字。《皇朝文鉴》卷一三九作‘京师里第’，今从之。〔二〕卫：原脱，据徐校、李刊本、《皇朝文鉴》补。〔三〕必颂宣尼：原作‘必以颂宣’，据李刊本、《皇朝文鉴》改。</t>
+          <t>君諱宣輔，字仲申。其先天水人也，累世從宦，不常厥居。曾祖全真，工部員外郎、滕州刺史。祖倚，太子校書。考臺，歙州海寧令。君即海寧府君第三子也，生于廣陵，長于江左。幼而俊敏，博綜羣書，尤善名法之學〔一〕。烈祖輔政，方申明紀律，君以是中選，釋褐補江都府文學，直刑部。明年，改信州司法參軍，察獄詳刑，號爲詳練。久之，召赴闕，以本官權參元帥府法曹事。踰年，改大理評事。元宗嗣服之初，精心庶獄，權要舉不附己者，因中傷之，君坐黜爲饒州司士參軍。明年，王師伐閩，護軍查公表君才可煩，使以本官判軍司事。時頓兵深入，自冬涉秋，經束馬懸車之塗，督飛芻輓粟之役，事集師尅，君有力焉。師還，加朝散大夫，行常州義興令，推誠率下，民用協和。丁憂去職，復爲江州録事參軍。時連帥議浚湓浦，以屯舟師，詔從之。君以無益戎備而勞民力，乃指陳利害，抗疏極論。上甚嘉之，即命止役。由是遷大理司直，通判蘄州軍州事。明年，遷檢校水部員外郎，充建州觀察推官，通判軍府事。會越人闚邊，使間誘建民，將以爲亂。君廉得其實，盡案誅之。優詔褒美，賜衣一襲，遷檢校屯田員外郎。三年，徵拜守水部員外郎，判度支。時師旅荐興，軍食不給，命君爲沿江催運使，軺傳所至，轉輸如流。朝議以姑熟居畿甸之間，實供億之始，徙君爲當塗令。踰月，復徵爲主客員外郎，判大理寺，賜紫金魚袋。始君以理官得罪，至是上知其無私，故復任焉。守官循理，挺然中立，轉工部員外郎，仍判寺事。今上嗣位，上疏論時政，以爲刺史縣令，親民之先，而考績掄材，未盡其理。上深然之，遷朝議大夫、戶部員外，充宣、歙、常、潤等道安撫使。以刺舉無避，爲權臣所排，宸鑑昭明，故得無咎。使還，以本官判兵部事。廬陵羣盗充斥，州兵不能制，上憂之，亟命君爲奉化軍節度判官，判吉州事，轉主客郎中，擒奸摘伏，克舉其職。其年秋九月七日遇暴疾，翌日終于郡之官舍，享年六十有一。明年春二月，歸葬江寧府某所，禮也。夫人查氏，吉王府長史昌之女、工部尚書文徽之妹。婉嬺之德，閨房之秀，內助著美，士林所推。子七人：長曰鈞，袁州新喻尉；次曰錯，樞密院承旨；次曰鍾，舉進士；次曰銓，前國子監三《禮》；次曰[CFont]NFCE5[/CFont]、鉞、鐭，皆國子監生。女一人，適秘書省正字周希定。君有孝悌之性，聞于宗族；敦然諾之信，稱于友朋。守己有常，事君不諂。位未達而知足，祿雖優而彌貧。其當官持事也，必盡己所長，不爲利回，不爲威惕，故屢失大臣意，然好直之士亦以此多之。鉉久塵近職，熟君操行，直筆聳善，以告後人，故銘其墓曰：英英趙君，松茂蘭薰。應用以法，飾身以文。道直詞正，心平氣純。如何不淑，今也爲塵。金陵仙鄉，古多名人。歸骨于是，與善爲鄰。泉臺不曉，壟樹空春。勒銘掛劍，慷慨霑巾。《徐公文集》卷一五。又見《全唐文》卷八八六。〔一〕名：原作‘身’，據《全唐文》、徐校、李校、四庫本改。</t>
         </is>
       </c>
       <c r="L10" t="n">
@@ -1029,41 +1013,37 @@
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
         <is>
-          <t>15;宋</t>
+          <t>6;唐</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4967237</t>
+          <t>4967201</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>42864</v>
+        <v>119793</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>易文赟</t>
+          <t>樊潛</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>广美</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>1</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>高安</t>
+          <t>貴池</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1072,33 +1052,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>府君讳文赟，字广美，豫章高安人也。在昔有晋，舂陵令雄〔一〕，位不充量，忠以亡身。祚流子孙〔二〕，繁衍荆楚。其世禄种德，则故老家牒详焉。曾祖暇、祖崇，皆不仕。妣邹氏，追封范阳县太君，从子贵也。君符彩爽迈，质性深沈，少遭时乱，静守家法，刚而无犯，勇而有节，乡曲之誉，蔼然于时。有吴功臣刘公信，节制豫章，训兵选士，闻君名而召之。君谓所亲曰：‘大丈夫当立功立事，以大家门。吾闻刘公刚毅倜傥，有英雄之量，必能申吾用也。’乃杖策从之，甚见器重。委以御侮，授之亲兵，出为爪牙，入参侍直，外捍封略，中清寇攘。十年之间，遂升右职。刘公物故，唐室中兴，君于是策名周行，入典离卫。于时戎事俯定，国容载穆，君止于拊循士众，恭守官常，时其寒燠，均其劳逸，勤毖邀道，廉察何留。不矜出位之思，甚得为将之体。自宣威军裨将，累迁至左右天威军都虞候〔三〕，自检校右常侍，至检校太保。及淮甸俶扰〔四〕，都邑震惊，以君为雄州刺史，充建武军使，其理所即广陵之天长县也。据冲要之地，有士民之众，绥怀训练，其俗用和。会周世宗亲总六师，志平江右，于是濠、泗携叛，扬、楚摧陷。君城小援绝，坚守累旬。世宗使降将郭廷谓临城招谕，君曰：‘弃命以茍生，不义；剿民以全名，不仁。吾处中道而已〔五〕。’乃间道表于本朝，备陈形势，且谕远虑。还旨嘉纳，谕以割地之谋。君即开城请罪，世宗慰劳数四，锡赉加等，即授衡州刺史，封太原县子，充天雄军节度行军司马。皇宋启运，优奖有加，改道州刺史，进爵为侯。君以俯绛老之年，有却克之疾，表求致仕，优诏不许。勤恳固请，听归临淮郡私第。春秋七十有五，开宝元年秋七月考终命。三年九月，葬于盱眙县义和乡西嵩里北团山，礼也。夫人会稽县君谢氏，亦江左之冠族。作合君子，克昭令仪。箴管之勤，夙彰于妇德；汤沐之邑，晚从于夫贵。训导诸子，备全义方。钟蓬首之痛，哀而知礼；受高堂之养，严而有慈。春秋七十有六，太平兴国二年秋七月，终于临淮私第。某年月日合祔焉，礼也。有子五人，曰延贵、延祚、延寿、延义，并克荷先业，勤修令名，或参藩郡，或干内职，皆先夫人而没。唯第四子延庆独禀粹和，服膺儒教，孝悌之至，称于州闾。承颜先意，侔曾、闵之行；居丧过哀，有二连之风。庐墓绝浆，义感生植，嘉木连理，玉芝成业。远近闻之，莫不惊叹。由是自前临淮令拜大理丞。及夫人卜葬，违制临赴，为有司所劾。有诏勿问，听解秩家居。惟府君之生也，临戎以恩信，理民以慈惠，事君全其节，处身由其道。故垂此家法，推为庆门，是生孝子，以永世祀，美矣哉!铉闻风而悦之，故勒铭于神道。其辞曰：于惟易氏，忠义之门。德厚流光，显于后昆。后昆之贤，生我府君。体道自居，壮图不群。辍耕永叹，负羽从军。赳赳和门，勇爵斯设。静则严重，动则奋发。临难忘私，处危全节。名遂身泰，考终无阙。芃芃泗川，永閟佳城。哀哀孝子，载感坤灵。君恩贲宠，乐石刊铭，百代之下，常流淑声。《徐公文集》卷二七。〔一〕舂陵：原作‘春陵’，据徐校、李刊本、四库本改。〔二〕祚：原作‘作’，据徐校、李刊本、四库本改。〔三〕累：原作‘异’，据徐校、黄校本、李刊本改。〔四〕陵：原作‘优’，据徐校、黄校本、李刊本改。〔五〕中：原作‘申’，据徐校、黄校本、李刊本、四库本改。</t>
+          <t>公諱潛，字仲明，京兆萬年人也。昔者虞仲垂孫謀之慶，肇啓我封；山甫昭補職之勤，實大吾族。或則游聖門而稱達者，或則冠仙籍而號真人〔一〕。豐沛功臣，經營于大業；南陽外戚，佐佑于中興。傳祀百世〔二〕，流光萬國。而我之占籍，世茂西京，樊川之居，抗衡韋、杜。曾祖澄，以七世同爨，孝德升聞，大中制恩，特加旌表，峨峨石闕，至今存焉。祖偁，濮州司戶參軍。考諭，光化中補池州至德令，時天下已亂，因家池陽，終潤州金壇令。公中和稟粹，形器夙成。好學之勤，本由天賦；至孝之性，不墜家聲。始及弱冠，併違怙恃。絶漿泣血，哀感州閭。負土成墳，終喪廬墓。言子道者，以爲美談。于時唐祚淪胥，宗室稱制，江淮之地，不失舊章。公以射策高等，補潤州丹陽尉，試吏之課，書考爲優。廬陵之民，古稱多訟，加以畝籍違制，亂獄滋豐。守臣上言，求拯其弊。有命擇堪其事者，聞公之能，因而命之。公既至，乃相五土之沃瘠，察夫家之衆寡，采古之制，酌今之宜，創爲新規，衆皆悅服。而復出械繫之者〔三〕，窮兩造之辭〔四〕，雪當死者數十人。使還議賞，增秩進等，遷壽州壽春縣主簿。既而廬陵之政日理，南楚之人聳觀。久之，以公爲光州光山縣令，加大理評事，猶以前效也。于時南北分裂，縣臨敵境，有爭桑之女，多探丸之吏〔五〕，比閭之衆，罕嘗寧居。公于是糾集義勇，分守要害，推以恩信，濟之強明，三載之中，一邑用乂。遷池州石埭令。縣有大姓，侵撓細民，歲比不登，俗乃重困。公繩之以法，董之以威，豪右震悚，相與逃匿。于是啓請出官粟以賑乏，絶省力役，以濟農功。慈撫仁薰，視之如子，歲豐俗阜，政用大成。就加大理司直，旌能政也。秩滿，遷鄂州漢陽令。未幾遇疾，壬子歲某月日，終于縣之正寢，享年五十有七。以丙辰歲某月日葬于池州貴池縣永泰鄉保靜里之原，禮也。夫人王氏，鴻臚卿滔之女。軒冕之族，閨房之秀，室家垂訓，惠問風行。長子若訥，不事王侯，自全高尚。次子知古，才藝畢給，際會昌朝，踐歷臺省，交修繁劇，今爲右諫議大夫、河北轉運使，揚名之業方茂，顯親之數遂優。公累贈秘書丞、戶部員外郎、衛尉少卿。夫人封瑯耶縣太君。惟公生而岐嶷，長而學問，窮九經之奧旨，綜百氏之微言。率是古道，施于爲政，行之以直，守之以廉，事親以孝，飾躬以禮。士元之器，命屈于生前；臧孫之忠，慶貽于身後。君恩飾壤，世祿傳家，咸京之舊表未堙，秋浦之豐碑復立，俗有遺愛，吾無愧辭。其銘曰：南山崇崇，樊川溶溶。翦商之烈，補袞之功。百代之後，流光不窮。爰有孝德，克生我公。猗歟我公，顯允君子。投此利刃，行于百里。有惠于民，何必貴仕；垂慶于後，何必在己!慶霄之澤，自葉流根。歿垂中佃，生駕魚軒。二子殊志，俱大吾門。僾僾愚谷，英英諫垣。九峰之下，貴池之口。覆斧馬鬣，金雞玉狗。民即桐鄉，碑如峴首。江水長流，令名同久。《徐公文集》卷二七。〔一〕仙：原作‘先’，據徐校、李刊本改。〔二〕祀：原作‘杞’，據徐校、黃校本、本刊本改。〔三〕‘者’字疑誤。〔四〕辭：原作‘亂’，據黃校本、李刊本改。〔五〕丸：原作‘九’，據徐校、黃校本、李刊本改。</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>7</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>刺史;道州;刺史;衡州;天雄军节度;裨将;军都虞候</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
         <v>1</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>延庆</t>
+          <t>知古</t>
         </is>
       </c>
       <c r="P11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>开宝</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr">
         <is>
           <t>15;宋</t>
@@ -1108,43 +1080,35 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4967253</t>
+          <t>4967204</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19635</v>
+        <v>36351</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>李从善</t>
+          <t>王煜</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>子师</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>开封;成纪</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>公讳从善，字子师，陇西成纪人。唐室之诸孙，元和之近属，谱谍详悉，此不具陈。若夫天祚之德，大运有时而极；积庆之祀，百世无得而逾。必生克肖之贤，以承有后之应。保姓受氏，公实宜之。昔者土德既微，群雄角立，维我显祖，奄宅旧吴，延祚四纪，傅国三世。公以天属之爱，膺宝玉之封。始在胶庠，已有名望。姿仪秀出，文学生知。仁孝极于事君，谦揖形于下士。中外之论，翕然称之。由是受任六官，交修庶职，弥纶旧典，咨访老成，恪居无违，所至皆理。于时圣人出于中土，正朔及于四方，维我先君，祇畏天命，受盟请吏，息民弭兵，玉帛交驰，冠盖相望。公亲则介弟，位则中台，独奉丝纶，留参槐棘。元戎驷牡，分建节之权；玄冕九章，奉侍祠之列。朝奖既厚，臣诚益恭。后凋之叶无渝，万顷之陂自若。故得全名节于危疑之际，保恩顾于终始之间。环卫迭迁，寄任增重，盘根必解，师律以真，十有余年，其志如一。呜呼!修涂方骋，景命不融，春秋四十有八，雍熙四年秋九月，薨于通许护军之廨。诏辍朝一日，赙绢百匹。即其年冬十月十三日葬于开封府开封县吹台乡苏里，祔太夫人凌氏之茔，礼也。前夫人徐氏，继室周氏，并早卒。皆有肃雍之德，窈窕之华，宜家治内尽其规，鱼轩象服昭其盛。子十四人：仲𫖮、仲翊、仲衍、仲华、仲雅、仲颖、仲宁、仲简、仲彬、仲文、仲猷、仲玄、仲义、仲端。女十四人：慕英、懿卿、奉苹、蕴兰、正容、茂节、稚仙、惠昭、如宾、道崇、凤兆、幼贞、闺秀、秀真，或嫔于盛族，或待礼未行。惟公生于深宫，特禀异气，谦而得礼，和而执中。容纳直言，宾延素士。经历夷险，雅度不渝，大年未登，终古同叹。铉登门斯久，辱顾殊深，永惟知己之恩，愿表为陵之谷。其铭曰：真源引派，仙李垂芳。实生我公，金玉其相。非礼勿动，出言有章。忠信以济，终然允臧。三代之姓，倏焉为庶；九万之程，溘然中路。吹台北峙，浚川东注。不植刺艸，长瞻宰树。大雅君子，陇西公之墓。《徐公文集》卷二九。</t>
+          <t>盛德百世，善繼者所以主其祀；聖人無外，善守者不能固其存。蓋運曆之所推，亦古今之一貫。其有享蕃錫之寵，保克終之美，殊恩飾壤，懿範流光，傳之金石，斯不誣矣。王諱煜，字重光，隴西人也。昔庭堅贊九德，伯陽恢至道。皇天眷祐，錫祚于唐，祖文宗武，世有顯德。載祀三百，龜玉淪胥，宗子維城，蕃衍萬國。江淮之地，獨奉長安，故我顯祖，用膺推戴。淳耀之烈，載光舊吳。二世承基，克廣其業。皇宋將啓，玄貺冥符。有周開先，太祖歷試。威德所及，寰宇將同。故我舊邦，祗畏天命，貶大號以稟朔，獻地圖而請吏。故得義動元后，風行域中，恩禮有加，綏懷不世。魯用天王之禮，自越常鈞；酅存紀侯之國，曾何足貴?王以世嫡嗣服，以古道馭民，欽若彝倫，率循先志。奉蒸嘗、恭色養必以孝，賓大臣、事耇老必以禮，居處服御必以節，言動施舍必以時。至于荷全濟之恩，謹藩國之度，勤修九貢，府無虛月，祗奉百役，知無不爲。十五年間，天眷彌渥。然而果于自信，怠于周防，西鄰起釁，南箕構禍。投杼致慈親之惑，乞火無里婦之辭。始勞因壘之師，終後塗山之會。太祖至仁之舉，大賚爲懷，録勤王之前效，恢焚謗之廣度，位以上將，爵爲通侯，待遇如初，寵錫斯厚。今上宣猷大麓，敷惠萬方，每侍論思，常存開釋。及飛天在運，麗澤推恩，擢進上公之封，仍加掌武之秩。侍從親禮，勉諭優容。方將度越等彝，登崇名數。嗚呼!閲川無捨，景命不融，太平興國三年秋七月八日遘疾，薨于京師里第〔一〕，享年四十有二。皇上撫几興悼，投瓜軫悲，痛生之不逮，俾歿而加飾，特詔輟朝三日，贈太師，追封吳王，命中使涖葬，凡喪祭所須，皆從官給。即其年冬十月日，葬于河南府某縣某鄉某里，禮也。夫人鄭國夫人周氏，勳舊之族，是生邦媛，肅雍之美，流詠國風，才實女師，言成閫則。子左千牛衛大將軍某〔二〕，襟神俊茂，識度淹通，孝悌自表于天資，才略靡由于師訓，日出之學，未易可量。惟王天骨秀異，神氣清粹。言動有則，容止可觀。精究六經，旁綜百氏。常以爲周、孔之道不可暫離，經國化民，發號施令，造次于是，終始不渝。酷好文辭，多所述作。一游一豫，必頌宣尼〔三〕；載笑載言，不忘經義。洞曉音律，精別雅鄭。窮先王制作之意，審風俗淳薄之原，爲文論之，以續《樂記》。所著文集三十卷，雜説百篇，味其文知其道矣。至于弧矢之善，筆札之工，天縱多能，必造精絶。本以惻隱之性，仍好竺乾之教，草木不殺，禽魚咸遂。賞人之善，常若不及；掩人之過，惟恐其聞。以至法不勝奸，威不克愛，以厭兵之俗，當用武之世。孔明罕應變之略，不成近功；偃王躬仁義之行，終于亡國。道有所在，復何愧歟?嗚呼哀哉!二室南峙，三川東注。瞻上陽之宮闕，望北邙之靈樹。旁寂寂兮迥野，下冥冥兮長暮。寄不朽于金石，庶有傳于竹素。其銘曰：天鑑九德，錫我唐祚。綿綿瓜瓞，茫茫商土。裔孫有慶，舊物重睹。開國承家，疆吳跨楚。喪亂孔棘，我恤疇依。聖人既作，我知所歸。終日靡俟，先天不違。惟藩惟輔，永言固之。道或汙隆，時有險易。蠅止于棘，虎游于市。明明大君，寬仁以濟。嘉爾前哲，釋茲後至。亦覯亦見，乃侯乃公。沐浴玄澤，徊翔景風。如松之茂，如山之崇。奈何不淑，運極化窮。舊國疏封，新阡啓室。人諗之謀，卜云其吉。龍章驥德，蘭言玉質。邈爾何往?此焉終畢。儼青蓋兮裶裶，驅素虬兮遲遲。即隧路兮徒返，望君門兮永辭。庶九原之可作，與緱嶺兮相期。垂斯文于億載，將樂石兮無虧。《徐公文集》卷二九。又見《皇朝文鑑》卷一三九。〔一〕京師里第：原作‘京師里之第’。徐校、李校云：‘師’下疑有脫字。《皇朝文鑑》卷一三九作‘京師里第’，今從之。〔二〕衛：原脫，據徐校、李刊本、《皇朝文鑑》補。〔三〕必頌宣尼：原作‘必以頌宣’，據李刊本、《皇朝文鑑》改。</t>
         </is>
       </c>
       <c r="L12" t="n">
@@ -1152,21 +1116,13 @@
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>仲翊</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>雍熙</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
           <t>15;宋</t>
@@ -1176,43 +1132,35 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4967269</t>
+          <t>4967204</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>39043</v>
+        <v>100865</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>王克贞</t>
+          <t>王煜</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>守节</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>庐陵</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>君讳克贞，字守节。其先太原人也。缑山之胄，本固源长；淮水既微，枝分派别。所居占籍，吴楚为多，今为庐陵人矣。曾祖某，不仕。祖某，赠吉州别驾。考某，屯田郎中。君弱不好弄，幼善属文，风骨峻整，器度闲雅，年未及冠，名闻于时。自唐室之季，词场道丧，江左延祚，复睹旧章。翰林学士江君文蔚典司春官，详求艺实，取人至寡，较文尤精。君一举擢第，首冠诸子，时人以为追踪元和之际矣。明年，以秘书省正字释褐，寓直枢近，专掌文翰之任。措词典雅，叙事详审，守位以慎，当官以勤。由是二十余年，累迁至中书舍人、枢密副使，未尝他任。求之前载，亦为异矣。及末叶多故，时政浸衰，唯吾守道中立，不涉浮议。及宗国沦丧，策名天朝，自太子中允，历户部、兵部二员外郎，礼部、户部二郎中，典汉、滑、襄、梓四州事。皆以宽简为务，仁爱推诚，当时之不名臣仆，长孺之择任丞史，是故民以之睦，政以之修。端拱二年秋，自梓潼还至京〔一〕，九月十八日，遘疾终于兴州之傅舍，享年六十。明年某月日，葬于扬州某县乡里，礼也。夫人陇西县君李氏，早亡。无子，女一人，许适盐铁使谏议陈某。惟君有文雅之用，有周慎之诚，言行相顾，光尘不异。奉职无废举，在私无惰容，历夷险而不回，保始终而无吝。初，君始从乡荐，余已典纶诰，谬为先达，屡辱请益。及余消长在运，而君金石不渝，古人之风，于是在矣。已悲深谷，更阅逝川，发为哀词，识彼泉户。铭曰：猗嗟夫君，心冥气纯。英英达士，亹亹词臣。不愆于位，有惠于民。无悔无咎，不缁不磷。吉往凶归，道悠运促。旋自九折，复于左毂。驷马悲鸣，市人行哭。邈矣彼苍，云何不淑!悠悠邗水〔二〕，隐隐昆冈。慈亲临奠，令季持丧。旁罗宰树，下閟玄堂。郊原掩霭，云日冥茫。痛光尘兮永已，念兰菊兮徒芳。《徐公文集》卷二九。〔一〕还至京：‘至’字疑衍。〔二〕邗：原作‘邦’，据徐校、李刊本改。</t>
+          <t>盛德百世，善繼者所以主其祀；聖人無外，善守者不能固其存。蓋運曆之所推，亦古今之一貫。其有享蕃錫之寵，保克終之美，殊恩飾壤，懿範流光，傳之金石，斯不誣矣。王諱煜，字重光，隴西人也。昔庭堅贊九德，伯陽恢至道。皇天眷祐，錫祚于唐，祖文宗武，世有顯德。載祀三百，龜玉淪胥，宗子維城，蕃衍萬國。江淮之地，獨奉長安，故我顯祖，用膺推戴。淳耀之烈，載光舊吳。二世承基，克廣其業。皇宋將啓，玄貺冥符。有周開先，太祖歷試。威德所及，寰宇將同。故我舊邦，祗畏天命，貶大號以稟朔，獻地圖而請吏。故得義動元后，風行域中，恩禮有加，綏懷不世。魯用天王之禮，自越常鈞；酅存紀侯之國，曾何足貴?王以世嫡嗣服，以古道馭民，欽若彝倫，率循先志。奉蒸嘗、恭色養必以孝，賓大臣、事耇老必以禮，居處服御必以節，言動施舍必以時。至于荷全濟之恩，謹藩國之度，勤修九貢，府無虛月，祗奉百役，知無不爲。十五年間，天眷彌渥。然而果于自信，怠于周防，西鄰起釁，南箕構禍。投杼致慈親之惑，乞火無里婦之辭。始勞因壘之師，終後塗山之會。太祖至仁之舉，大賚爲懷，録勤王之前效，恢焚謗之廣度，位以上將，爵爲通侯，待遇如初，寵錫斯厚。今上宣猷大麓，敷惠萬方，每侍論思，常存開釋。及飛天在運，麗澤推恩，擢進上公之封，仍加掌武之秩。侍從親禮，勉諭優容。方將度越等彝，登崇名數。嗚呼!閲川無捨，景命不融，太平興國三年秋七月八日遘疾，薨于京師里第〔一〕，享年四十有二。皇上撫几興悼，投瓜軫悲，痛生之不逮，俾歿而加飾，特詔輟朝三日，贈太師，追封吳王，命中使涖葬，凡喪祭所須，皆從官給。即其年冬十月日，葬于河南府某縣某鄉某里，禮也。夫人鄭國夫人周氏，勳舊之族，是生邦媛，肅雍之美，流詠國風，才實女師，言成閫則。子左千牛衛大將軍某〔二〕，襟神俊茂，識度淹通，孝悌自表于天資，才略靡由于師訓，日出之學，未易可量。惟王天骨秀異，神氣清粹。言動有則，容止可觀。精究六經，旁綜百氏。常以爲周、孔之道不可暫離，經國化民，發號施令，造次于是，終始不渝。酷好文辭，多所述作。一游一豫，必頌宣尼〔三〕；載笑載言，不忘經義。洞曉音律，精別雅鄭。窮先王制作之意，審風俗淳薄之原，爲文論之，以續《樂記》。所著文集三十卷，雜説百篇，味其文知其道矣。至于弧矢之善，筆札之工，天縱多能，必造精絶。本以惻隱之性，仍好竺乾之教，草木不殺，禽魚咸遂。賞人之善，常若不及；掩人之過，惟恐其聞。以至法不勝奸，威不克愛，以厭兵之俗，當用武之世。孔明罕應變之略，不成近功；偃王躬仁義之行，終于亡國。道有所在，復何愧歟?嗚呼哀哉!二室南峙，三川東注。瞻上陽之宮闕，望北邙之靈樹。旁寂寂兮迥野，下冥冥兮長暮。寄不朽于金石，庶有傳于竹素。其銘曰：天鑑九德，錫我唐祚。綿綿瓜瓞，茫茫商土。裔孫有慶，舊物重睹。開國承家，疆吳跨楚。喪亂孔棘，我恤疇依。聖人既作，我知所歸。終日靡俟，先天不違。惟藩惟輔，永言固之。道或汙隆，時有險易。蠅止于棘，虎游于市。明明大君，寬仁以濟。嘉爾前哲，釋茲後至。亦覯亦見，乃侯乃公。沐浴玄澤，徊翔景風。如松之茂，如山之崇。奈何不淑，運極化窮。舊國疏封，新阡啓室。人諗之謀，卜云其吉。龍章驥德，蘭言玉質。邈爾何往?此焉終畢。儼青蓋兮裶裶，驅素虬兮遲遲。即隧路兮徒返，望君門兮永辭。庶九原之可作，與緱嶺兮相期。垂斯文于億載，將樂石兮無虧。《徐公文集》卷二九。又見《皇朝文鑑》卷一三九。〔一〕京師里第：原作‘京師里之第’。徐校、李校云：‘師’下疑有脫字。《皇朝文鑑》卷一三九作‘京師里第’，今從之。〔二〕衛：原脫，據徐校、李刊本、《皇朝文鑑》補。〔三〕必頌宣尼：原作‘必以頌宣’，據李刊本、《皇朝文鑑》改。</t>
         </is>
       </c>
       <c r="L13" t="n">
@@ -1224,31 +1172,27 @@
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>端拱</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr">
         <is>
-          <t>15;宋</t>
+          <t>18;元</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4967277</t>
+          <t>4967237</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>39436</v>
+        <v>42864</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>江直木</t>
+          <t>易文贇</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1259,40 +1203,48 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>子建</t>
+          <t>廣美</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>高安</t>
+        </is>
+      </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>君讳直木，字子建，寻阳人也。庐九之地，时生俊才；忠壮之族，世著南国。末叶湮替，与时污隆，儒、墨退让，垂为家法。曾祖晁、祖𧏖、考骘，皆不仕。伯父梦孙，与先君同隐庐山，以经学大义自娱。伯父后膺宰府之辟〔一〕，自求弦歌之任，报政罢去，复隐旧山，孝友贞清，乡里推服。先妣李氏方娠，梦神人授以直木一本，寤而生君，故取名焉。幼而颖悟，生知经义，七岁以神童擢第。未几，丁先君忧，至性孺慕，宗族称叹，孜孜色养，无复宦情。学古属文，惟日不足，爰及弱冠，遂以词艺知名。其为文清淡简约，自为品格，尤长于古风诗。家居凡二十五年，亲友惇喻，乃从常调，释褐太常寺奉礼郎，转江都县主簿。直以事上，不失其恭；勤以率下，毕举其职。民从其化，吏服其能。府尹陈玄藻、县令路仪，皆恃才傲物，独推重于君，以为不如也。改江夏令，其理如初。鄂帅何洙，武勋致位，性复暴桀，亦加优礼，异于余人。尝视君举止迂缓，车服朴野，辄怡然而笑，每责诸寮属曰：‘君辈称为儒生，不学江令也!’秩满，改蕲州黄梅令，议者以为屈，君以乡曲俯接，欣然而往。逾岁，迁歙州黟县令。会宗属封建，妙选府寮，授君记室之任。处平台复道之地，列玳簪珠履之间，清节素风，凛然不改，正词直道，动必尽规，府公甚重之。十有余年，累迁至水部员外郎，赐绯，而记室如故。庚午岁，府公奉使天朝，留镇兖海，授君泰宁节度判官、检校金部员外郎。数年，迁司门员外郎，判刑部。今上元年，加朝奉郎，先君赠大理司直，先妣追封陇西县太君。视事三载，求外任以自效。上以君恭勤详慎，宜久其职，拜兵部员外郎，仍兼刑部。享年六十有四。居常康宁，微病数日，奄从物故，时太平兴国五年冬十二月二十八日也。即明年二月十日，葬于开封县汴阳乡丰台里，礼也。前夫人封氏、今夫人太原县君王氏，皆有窈窕之质，幽闲之操，叶此贞节，蔚其门风。长子敞，京兆府醴泉县主簿。次曰用成、用明、用澄、用康、用平、用文、用宁。女二人，曰慕昭、用贞。君生于季俗，世全素业，性纯貌古，行洁文高，守道安贫，非礼不动，未尝忤物，亦不随流，真所谓鞠躬君子者矣。夙惠之性，禀于天资。年十余岁，侍伯父食，不过园疏而已。伯父戏之曰：‘啜白薤之羹，淡而无味。’君应声答曰：‘啮紫茄之蒂，铿尔有声。’人知其当大成也。余始闻其名，晚乃识面，察言观行，重其为人。藩房见选，余所荐也，亦既称职，颇尝自多。丙寅岁与君具年五十岁，日会饮酒，相与赋诗，君先就，曰：‘学《易》宁无道?知非素有心。’余遂不复作也。君有文集二十卷。呜呼!契阔夷险，咨嗟年鬓，一生一死，孰克忘情!聊存挂剑之稘，故有刊铭之作。其词曰：呜呼江君，世济其名。生今之俗，为古之人。闺门侃侃，乡里恂恂。其实如秋，其华如春。握兰有裕，伏阁惟勤。考终归全，邈焉清尘。葬于所没，古称达者。浚水长源，夷门迥野。徒挂宝剑，空驰白马。胜气如存，逝川不舍。勒石垂芳，千载之下。《徐公文集》卷二九。〔一〕辟：原作‘辞’，据徐校、李刊本改。</t>
+          <t>府君諱文贇，字廣美，豫章高安人也。在昔有晉，舂陵令雄〔一〕，位不充量，忠以亡身。祚流子孫〔二〕，繁衍荊楚。其世祿種德，則故老家牒詳焉。曾祖暇、祖崇，皆不仕。妣鄒氏，追封范陽縣太君，從子貴也。君符彩爽邁，質性深沉，少遭時亂，靜守家法，剛而無犯，勇而有節，鄉曲之譽，藹然于時。有吳功臣劉公信，節制豫章，訓兵選士，聞君名而召之。君謂所親曰：‘大丈夫當立功立事，以大家門。吾聞劉公剛毅倜儻，有英雄之量，必能申吾用也。’乃杖策從之，甚見器重。委以御侮，授之親兵，出爲爪牙，入參侍直，外捍封略，中清寇攘。十年之間，遂升右職。劉公物故，唐室中興，君于是策名周行，入典離衛。于時戎事俯定，國容載穆，君止于拊循士衆，恭守官常，時其寒燠，均其勞逸，勤毖徼道，廉察何留。不矜出位之思，甚得爲將之體。自宣威軍裨將，累遷至左右天威軍都虞候〔三〕，自檢校右常侍，至檢校太保。及淮甸俶擾〔四〕，都邑震驚，以君爲雄州刺史，充建武軍使，其理所即廣陵之天長縣也。據沖要之地，有士民之衆，綏懷訓練，其俗用和。會周世宗親總六師，志平江右，于是濠、泗攜叛，揚、楚摧陷。君城小援絶，堅守累旬。世宗使降將郭廷謂臨城招諭，君曰：‘棄命以茍生，不義；剿民以全名，不仁。吾處中道而已〔五〕。’乃間道表于本朝，備陳形勢，且諭遠慮。還旨嘉納，諭以割地之謀。君即開城請罪，世宗慰勞數四，錫賚加等，即授衡州刺史，封太原縣子，充天雄軍節度行軍司馬。皇宋啓運，優奬有加，改道州刺史，進爵爲侯。君以俯絳老之年，有郤克之疾，表求致仕，優詔不許。勤懇固請，聽歸臨淮郡私第。春秋七十有五，開寶元年秋七月考終命。三年九月，葬于盱眙縣義和鄉西嵩里北團山，禮也。夫人會稽縣君謝氏，亦江左之冠族。作合君子，克昭令儀。箴管之勤，夙彰于婦德；湯沐之邑，晚從于夫貴。訓導諸子，備全義方。鍾蓬首之痛，哀而知禮；受高堂之養，嚴而有慈。春秋七十有六，太平興國二年秋七月，終于臨淮私第。某年月日合祔焉，禮也。有子五人，曰延貴、延祚、延壽、延義，並克荷先業，勤修令名，或參藩郡，或幹內職，皆先夫人而沒。唯第四子延慶獨稟粹和，服膺儒教，孝悌之至，稱于州閭。承顔先意，侔曾、閔之行；居喪過哀，有二連之風。廬墓絶漿，義感生植，嘉木連理，玉芝成業。遠近聞之，莫不驚歎。由是自前臨淮令拜大理丞。及夫人卜葬，違制臨赴，爲有司所劾。有詔勿問，聽解秩家居。惟府君之生也，臨戎以恩信，理民以慈惠，事君全其節，處身由其道。故垂此家法，推爲慶門，是生孝子，以永世祀，美矣哉!鉉聞風而悅之，故勒銘于神道。其辭曰：於惟易氏，忠義之門。德厚流光，顯于後昆。後昆之賢，生我府君。體道自居，壯圖不群。輟耕永歎，負羽從軍。赳赳和門，勇爵斯設。靜則嚴重，動則奮發。臨難忘私，處危全節。名遂身泰，考終無闕。芃芃泗川，永閟佳城。哀哀孝子，載感坤靈。君恩賁寵，樂石刊銘，百代之下，常流淑聲。《徐公文集》卷二七。〔一〕舂陵：原作‘春陵’，據徐校、李刊本、四庫本改。〔二〕祚：原作‘作’，據徐校、李刊本、四庫本改。〔三〕累：原作‘異’，據徐校、黃校本、李刊本改。〔四〕陵：原作‘優’，據徐校、黃校本、李刊本改。〔五〕中：原作‘申’，據徐校、黃校本、李刊本、四庫本改。</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>太常寺奉礼郎;太常寺奉礼郎;县令;江夏;县令;黄梅;县令;县主簿;江都</t>
+          <t>刺史;道州;刺史;衡州;天雄軍節度;裨將;軍都虞候</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>延慶</t>
+        </is>
+      </c>
       <c r="P14" t="n">
         <v>1</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>太平兴国</t>
+          <t>開寶</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1304,35 +1256,43 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1762</t>
+          <t>4967253</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1762</v>
+        <v>19635</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>王安石</t>
+          <t>李從善</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>子師</t>
+        </is>
+      </c>
       <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>開封;成紀</t>
+        </is>
+      </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>进士举人测试</t>
+          <t>公諱從善，字子師，隴西成紀人。唐室之諸孫，元和之近屬，譜諜詳悉，此不具陳。若夫天祚之德，大運有時而極；積慶之祀，百世無得而逾。必生克肖之賢，以承有後之應。保姓受氏，公實宜之。昔者土德既微，群雄角立，維我顯祖，奄宅舊吴，延祚四紀，傳國三世。公以天屬之愛，膺寶玉之封。始在膠庠，已有名望。姿儀秀出，文學生知。仁孝極于事君，謙揖形于下士。中外之論，翕然稱之。由是受任六官，交修庶職，彌綸舊典，諮訪老成，恪居無違，所至皆理。于時聖人出于中土，正朔及于四方，維我先君，祗畏天命，受盟請吏，息民弭兵，玉帛交馳，冠蓋相望。公親則介弟，位則中台，獨奉絲綸，留參槐棘。元戎駟牡，分建節之權；玄冕九章，奉侍祠之列。朝奬既厚，臣誠益恭。後凋之葉無渝，萬頃之陂自若。故得全名節于危疑之際，保恩顧于終始之間。環衛迭遷，寄任增重，盤根必解，師律以真，十有餘年，其志如一。嗚呼!修塗方騁，景命不融，春秋四十有八，雍熙四年秋九月，薨于通許護軍之廨。詔輟朝一日，賻絹百匹。即其年冬十月十三日葬于開封府開封縣吹臺鄉蘇里，祔太夫人凌氏之塋，禮也。前夫人徐氏，繼室周氏，並早卒。皆有肅雍之德，窈窕之華，宜家治內盡其規，魚軒象服昭其盛。子十四人：仲顗、仲翊、仲衍、仲華、仲雅、仲穎、仲寧、仲簡、仲彬、仲文、仲猷、仲玄、仲義、仲端。女十四人：慕英、懿卿、奉蘋、藴蘭、正容、茂節、穉仙、惠昭、如賓、道崇、鳳兆、幼貞、閨秀、秀真，或嬪于盛族，或待禮未行。惟公生于深宮，特禀異氣，謙而得禮，和而執中。容納直言，賓延素士。經歷夷險，雅度不渝，大年未登，終古同歎。鉉登門斯久，辱顧殊深，永惟知己之恩，願表爲陵之谷。其銘曰：真源引派，仙李垂芳。實生我公，金玉其相。非禮勿動，出言有章。忠信以濟，終然允臧。三代之姓，倏焉爲庶；九萬之程，溘然中路。吹臺北峙，浚川東注。不植刺草，長瞻宰樹。大雅君子，隴西公之墓。《徐公文集》卷二九。</t>
         </is>
       </c>
       <c r="L15" t="n">
@@ -1340,14 +1300,470 @@
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>仲翊</t>
+        </is>
+      </c>
       <c r="P15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>雍熙</t>
+        </is>
+      </c>
       <c r="R15" t="inlineStr">
+        <is>
+          <t>15;宋</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>4967253</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>103369</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>李從善</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>公諱從善，字子師，隴西成紀人。唐室之諸孫，元和之近屬，譜諜詳悉，此不具陳。若夫天祚之德，大運有時而極；積慶之祀，百世無得而逾。必生克肖之賢，以承有後之應。保姓受氏，公實宜之。昔者土德既微，群雄角立，維我顯祖，奄宅舊吴，延祚四紀，傳國三世。公以天屬之愛，膺寶玉之封。始在膠庠，已有名望。姿儀秀出，文學生知。仁孝極于事君，謙揖形于下士。中外之論，翕然稱之。由是受任六官，交修庶職，彌綸舊典，諮訪老成，恪居無違，所至皆理。于時聖人出于中土，正朔及于四方，維我先君，祗畏天命，受盟請吏，息民弭兵，玉帛交馳，冠蓋相望。公親則介弟，位則中台，獨奉絲綸，留參槐棘。元戎駟牡，分建節之權；玄冕九章，奉侍祠之列。朝奬既厚，臣誠益恭。後凋之葉無渝，萬頃之陂自若。故得全名節于危疑之際，保恩顧于終始之間。環衛迭遷，寄任增重，盤根必解，師律以真，十有餘年，其志如一。嗚呼!修塗方騁，景命不融，春秋四十有八，雍熙四年秋九月，薨于通許護軍之廨。詔輟朝一日，賻絹百匹。即其年冬十月十三日葬于開封府開封縣吹臺鄉蘇里，祔太夫人凌氏之塋，禮也。前夫人徐氏，繼室周氏，並早卒。皆有肅雍之德，窈窕之華，宜家治內盡其規，魚軒象服昭其盛。子十四人：仲顗、仲翊、仲衍、仲華、仲雅、仲穎、仲寧、仲簡、仲彬、仲文、仲猷、仲玄、仲義、仲端。女十四人：慕英、懿卿、奉蘋、藴蘭、正容、茂節、穉仙、惠昭、如賓、道崇、鳳兆、幼貞、閨秀、秀真，或嬪于盛族，或待禮未行。惟公生于深宮，特禀異氣，謙而得禮，和而執中。容納直言，賓延素士。經歷夷險，雅度不渝，大年未登，終古同歎。鉉登門斯久，辱顧殊深，永惟知己之恩，願表爲陵之谷。其銘曰：真源引派，仙李垂芳。實生我公，金玉其相。非禮勿動，出言有章。忠信以濟，終然允臧。三代之姓，倏焉爲庶；九萬之程，溘然中路。吹臺北峙，浚川東注。不植刺草，長瞻宰樹。大雅君子，隴西公之墓。《徐公文集》卷二九。</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>18;元</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>4967253</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>103370</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>李從善</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>公諱從善，字子師，隴西成紀人。唐室之諸孫，元和之近屬，譜諜詳悉，此不具陳。若夫天祚之德，大運有時而極；積慶之祀，百世無得而逾。必生克肖之賢，以承有後之應。保姓受氏，公實宜之。昔者土德既微，群雄角立，維我顯祖，奄宅舊吴，延祚四紀，傳國三世。公以天屬之愛，膺寶玉之封。始在膠庠，已有名望。姿儀秀出，文學生知。仁孝極于事君，謙揖形于下士。中外之論，翕然稱之。由是受任六官，交修庶職，彌綸舊典，諮訪老成，恪居無違，所至皆理。于時聖人出于中土，正朔及于四方，維我先君，祗畏天命，受盟請吏，息民弭兵，玉帛交馳，冠蓋相望。公親則介弟，位則中台，獨奉絲綸，留參槐棘。元戎駟牡，分建節之權；玄冕九章，奉侍祠之列。朝奬既厚，臣誠益恭。後凋之葉無渝，萬頃之陂自若。故得全名節于危疑之際，保恩顧于終始之間。環衛迭遷，寄任增重，盤根必解，師律以真，十有餘年，其志如一。嗚呼!修塗方騁，景命不融，春秋四十有八，雍熙四年秋九月，薨于通許護軍之廨。詔輟朝一日，賻絹百匹。即其年冬十月十三日葬于開封府開封縣吹臺鄉蘇里，祔太夫人凌氏之塋，禮也。前夫人徐氏，繼室周氏，並早卒。皆有肅雍之德，窈窕之華，宜家治內盡其規，魚軒象服昭其盛。子十四人：仲顗、仲翊、仲衍、仲華、仲雅、仲穎、仲寧、仲簡、仲彬、仲文、仲猷、仲玄、仲義、仲端。女十四人：慕英、懿卿、奉蘋、藴蘭、正容、茂節、穉仙、惠昭、如賓、道崇、鳳兆、幼貞、閨秀、秀真，或嬪于盛族，或待禮未行。惟公生于深宮，特禀異氣，謙而得禮，和而執中。容納直言，賓延素士。經歷夷險，雅度不渝，大年未登，終古同歎。鉉登門斯久，辱顧殊深，永惟知己之恩，願表爲陵之谷。其銘曰：真源引派，仙李垂芳。實生我公，金玉其相。非禮勿動，出言有章。忠信以濟，終然允臧。三代之姓，倏焉爲庶；九萬之程，溘然中路。吹臺北峙，浚川東注。不植刺草，長瞻宰樹。大雅君子，隴西公之墓。《徐公文集》卷二九。</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>18;元</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4967253</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>103371</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>李從善</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>公諱從善，字子師，隴西成紀人。唐室之諸孫，元和之近屬，譜諜詳悉，此不具陳。若夫天祚之德，大運有時而極；積慶之祀，百世無得而逾。必生克肖之賢，以承有後之應。保姓受氏，公實宜之。昔者土德既微，群雄角立，維我顯祖，奄宅舊吴，延祚四紀，傳國三世。公以天屬之愛，膺寶玉之封。始在膠庠，已有名望。姿儀秀出，文學生知。仁孝極于事君，謙揖形于下士。中外之論，翕然稱之。由是受任六官，交修庶職，彌綸舊典，諮訪老成，恪居無違，所至皆理。于時聖人出于中土，正朔及于四方，維我先君，祗畏天命，受盟請吏，息民弭兵，玉帛交馳，冠蓋相望。公親則介弟，位則中台，獨奉絲綸，留參槐棘。元戎駟牡，分建節之權；玄冕九章，奉侍祠之列。朝奬既厚，臣誠益恭。後凋之葉無渝，萬頃之陂自若。故得全名節于危疑之際，保恩顧于終始之間。環衛迭遷，寄任增重，盤根必解，師律以真，十有餘年，其志如一。嗚呼!修塗方騁，景命不融，春秋四十有八，雍熙四年秋九月，薨于通許護軍之廨。詔輟朝一日，賻絹百匹。即其年冬十月十三日葬于開封府開封縣吹臺鄉蘇里，祔太夫人凌氏之塋，禮也。前夫人徐氏，繼室周氏，並早卒。皆有肅雍之德，窈窕之華，宜家治內盡其規，魚軒象服昭其盛。子十四人：仲顗、仲翊、仲衍、仲華、仲雅、仲穎、仲寧、仲簡、仲彬、仲文、仲猷、仲玄、仲義、仲端。女十四人：慕英、懿卿、奉蘋、藴蘭、正容、茂節、穉仙、惠昭、如賓、道崇、鳳兆、幼貞、閨秀、秀真，或嬪于盛族，或待禮未行。惟公生于深宮，特禀異氣，謙而得禮，和而執中。容納直言，賓延素士。經歷夷險，雅度不渝，大年未登，終古同歎。鉉登門斯久，辱顧殊深，永惟知己之恩，願表爲陵之谷。其銘曰：真源引派，仙李垂芳。實生我公，金玉其相。非禮勿動，出言有章。忠信以濟，終然允臧。三代之姓，倏焉爲庶；九萬之程，溘然中路。吹臺北峙，浚川東注。不植刺草，長瞻宰樹。大雅君子，隴西公之墓。《徐公文集》卷二九。</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>18;元</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>4967253</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>103372</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>李從善</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>公諱從善，字子師，隴西成紀人。唐室之諸孫，元和之近屬，譜諜詳悉，此不具陳。若夫天祚之德，大運有時而極；積慶之祀，百世無得而逾。必生克肖之賢，以承有後之應。保姓受氏，公實宜之。昔者土德既微，群雄角立，維我顯祖，奄宅舊吴，延祚四紀，傳國三世。公以天屬之愛，膺寶玉之封。始在膠庠，已有名望。姿儀秀出，文學生知。仁孝極于事君，謙揖形于下士。中外之論，翕然稱之。由是受任六官，交修庶職，彌綸舊典，諮訪老成，恪居無違，所至皆理。于時聖人出于中土，正朔及于四方，維我先君，祗畏天命，受盟請吏，息民弭兵，玉帛交馳，冠蓋相望。公親則介弟，位則中台，獨奉絲綸，留參槐棘。元戎駟牡，分建節之權；玄冕九章，奉侍祠之列。朝奬既厚，臣誠益恭。後凋之葉無渝，萬頃之陂自若。故得全名節于危疑之際，保恩顧于終始之間。環衛迭遷，寄任增重，盤根必解，師律以真，十有餘年，其志如一。嗚呼!修塗方騁，景命不融，春秋四十有八，雍熙四年秋九月，薨于通許護軍之廨。詔輟朝一日，賻絹百匹。即其年冬十月十三日葬于開封府開封縣吹臺鄉蘇里，祔太夫人凌氏之塋，禮也。前夫人徐氏，繼室周氏，並早卒。皆有肅雍之德，窈窕之華，宜家治內盡其規，魚軒象服昭其盛。子十四人：仲顗、仲翊、仲衍、仲華、仲雅、仲穎、仲寧、仲簡、仲彬、仲文、仲猷、仲玄、仲義、仲端。女十四人：慕英、懿卿、奉蘋、藴蘭、正容、茂節、穉仙、惠昭、如賓、道崇、鳳兆、幼貞、閨秀、秀真，或嬪于盛族，或待禮未行。惟公生于深宮，特禀異氣，謙而得禮，和而執中。容納直言，賓延素士。經歷夷險，雅度不渝，大年未登，終古同歎。鉉登門斯久，辱顧殊深，永惟知己之恩，願表爲陵之谷。其銘曰：真源引派，仙李垂芳。實生我公，金玉其相。非禮勿動，出言有章。忠信以濟，終然允臧。三代之姓，倏焉爲庶；九萬之程，溘然中路。吹臺北峙，浚川東注。不植刺草，長瞻宰樹。大雅君子，隴西公之墓。《徐公文集》卷二九。</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>18;元</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>4967253</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>488731</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>李從善</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>公諱從善，字子師，隴西成紀人。唐室之諸孫，元和之近屬，譜諜詳悉，此不具陳。若夫天祚之德，大運有時而極；積慶之祀，百世無得而逾。必生克肖之賢，以承有後之應。保姓受氏，公實宜之。昔者土德既微，群雄角立，維我顯祖，奄宅舊吴，延祚四紀，傳國三世。公以天屬之愛，膺寶玉之封。始在膠庠，已有名望。姿儀秀出，文學生知。仁孝極于事君，謙揖形于下士。中外之論，翕然稱之。由是受任六官，交修庶職，彌綸舊典，諮訪老成，恪居無違，所至皆理。于時聖人出于中土，正朔及于四方，維我先君，祗畏天命，受盟請吏，息民弭兵，玉帛交馳，冠蓋相望。公親則介弟，位則中台，獨奉絲綸，留參槐棘。元戎駟牡，分建節之權；玄冕九章，奉侍祠之列。朝奬既厚，臣誠益恭。後凋之葉無渝，萬頃之陂自若。故得全名節于危疑之際，保恩顧于終始之間。環衛迭遷，寄任增重，盤根必解，師律以真，十有餘年，其志如一。嗚呼!修塗方騁，景命不融，春秋四十有八，雍熙四年秋九月，薨于通許護軍之廨。詔輟朝一日，賻絹百匹。即其年冬十月十三日葬于開封府開封縣吹臺鄉蘇里，祔太夫人凌氏之塋，禮也。前夫人徐氏，繼室周氏，並早卒。皆有肅雍之德，窈窕之華，宜家治內盡其規，魚軒象服昭其盛。子十四人：仲顗、仲翊、仲衍、仲華、仲雅、仲穎、仲寧、仲簡、仲彬、仲文、仲猷、仲玄、仲義、仲端。女十四人：慕英、懿卿、奉蘋、藴蘭、正容、茂節、穉仙、惠昭、如賓、道崇、鳳兆、幼貞、閨秀、秀真，或嬪于盛族，或待禮未行。惟公生于深宮，特禀異氣，謙而得禮，和而執中。容納直言，賓延素士。經歷夷險，雅度不渝，大年未登，終古同歎。鉉登門斯久，辱顧殊深，永惟知己之恩，願表爲陵之谷。其銘曰：真源引派，仙李垂芳。實生我公，金玉其相。非禮勿動，出言有章。忠信以濟，終然允臧。三代之姓，倏焉爲庶；九萬之程，溘然中路。吹臺北峙，浚川東注。不植刺草，長瞻宰樹。大雅君子，隴西公之墓。《徐公文集》卷二九。</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>18;元</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>4967269</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>39043</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>王克貞</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>守節</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>廬陵</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>君諱克貞，字守節。其先太原人也。緱山之胄，本固源長；淮水既微，枝分派别。所居占籍，吴楚爲多，今爲廬陵人矣。曾祖某，不仕。祖某，贈吉州別駕。考某，屯田郎中。君弱不好弄，幼善屬文，風骨峻整，器度閑雅，年未及冠，名聞于時。自唐室之季，詞場道喪，江左延祚，復覩舊章。翰林學士江君文蔚典司春官，詳求藝實，取人至寡，較文尤精。君一舉擢第，首冠諸子，時人以爲追蹤元和之際矣。明年，以秘書省正字釋褐，寓直樞近，專掌文翰之任。措詞典雅，敘事詳審，守位以慎，當官以勤。由是二十餘年，累遷至中書舍人、樞密副使，未嘗他任。求之前載，亦爲異矣。及末葉多故，時政浸衰，唯吾守道中立，不涉浮議。及宗國淪喪，策名天朝，自太子中允，歷戶部、兵部二員外郎，禮部、戶部二郎中，典漢、滑、襄、梓四州事。皆以寬簡爲務，仁愛推誠，當時之不名臣僕，長孺之擇任丞史，是故民以之睦，政以之修。端拱二年秋，自梓潼還至京〔一〕，九月十八日，遘疾終于興州之傳舍，享年六十。明年某月日，葬于揚州某縣鄉里，禮也。夫人隴西縣君李氏，早亡。無子，女一人，許適鹽鐵使諫議陳某。惟君有文雅之用，有周慎之誠，言行相顧，光塵不異。奉職無廢舉，在私無惰容，歷夷險而不回，保始終而無吝。初，君始從鄉薦，余已典綸誥，謬爲先達，屢辱請益。及余消長在運，而君金石不渝，古人之風，于是在矣。已悲深谷，更閲逝川，發爲哀詞，識彼泉戶。銘曰：猗嗟夫君，心冥氣純。英英達士，亹亹詞臣。不愆于位，有惠于民。無悔無咎，不緇不磷。吉往兇歸，道悠運促。旋自九折，復于左轂。駟馬悲鳴，市人行哭。邈矣彼蒼，云何不淑!悠悠邗水〔二〕，隱隱崑岡。慈親臨奠，令季持喪。旁羅宰樹，下閟玄堂。郊原掩靄，雲日冥茫。痛光塵兮永已，念蘭菊兮徒芳。《徐公文集》卷二九。〔一〕還至京：‘至’字疑衍。〔二〕邗：原作‘邦’，據徐校、李刊本改。</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>端拱</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>15;宋</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>4967277</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>39436</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>江直木</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>11</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>子建</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>君諱直木，字子建，尋陽人也。廬九之地，時生俊才；忠壯之族，世著南國。末葉湮替，與時汙隆，儒、墨退讓，垂爲家法。曾祖晁、祖蠙、考隲，皆不仕。伯父夢孫，與先君同隱廬山，以經學大義自娛。伯父後膺宰府之辟〔一〕，自求弦歌之任，報政罷去，復隱舊山，孝友貞清，鄉里推服。先妣李氏方娠，夢神人授以直木一本，寤而生君，故取名焉。幼而穎悟，生知經義，七歲以神童擢第。未幾，丁先君憂，至性孺慕，宗族稱歎，孜孜色養，無復宦情。學古屬文，惟日不足，爰及弱冠，遂以詞藝知名。其爲文清淡簡約，自爲品格，尤長于古風詩。家居凡二十五年，親友敦喻，乃從常調，釋褐太常寺奉禮郎，轉江都縣主簿。直以事上，不失其恭；勤以率下，畢舉其職。民從其化，吏服其能。府尹陳玄藻、縣令路儀，皆恃才傲物，獨推重于君，以爲不如也。改江夏令，其理如初。鄂帥何洙，武勳致位，性復暴桀，亦加優禮，異于餘人。嘗視君舉止迂緩，車服樸野，輒怡然而笑，每責諸寮屬曰：‘君輩稱爲儒生，不學江令也!’秩滿，改蘄州黃梅令，議者以爲屈，君以鄉曲俯接，欣然而往。逾歲，遷歙州黟縣令。會宗屬封建，妙選府寮，授君記室之任。處平臺複道之地，列瑇簪珠履之間，清節素風，凜然不改，正詞直道，動必盡規，府公甚重之。十有餘年，累遷至水部員外郎，賜緋，而記室如故。庚午歲，府公奉使天朝，留鎮兗海，授君泰寧節度判官、檢校金部員外郎。數年，遷司門員外郎，判刑部。今上元年，加朝奉郎，先君贈大理司直，先妣追封隴西縣太君。視事三載，求外任以自效。上以君恭勤詳慎，宜久其職，拜兵部員外郎，仍兼刑部。享年六十有四。居常康寧，微病數日，奄從物故，時太平興國五年冬十二月二十八日也。即明年二月十日，葬于開封縣汴陽鄉豐臺里，禮也。前夫人封氏、今夫人太原縣君王氏，皆有窈窕之質，幽閑之操，叶此貞節，蔚其門風。長子敞，京兆府醴泉縣主簿。次曰用成、用明、用澄、用康、用平、用文、用寧。女二人，曰慕昭、用貞。君生于季俗，世全素業，性純貌古，行潔文高，守道安貧，非禮不動，未嘗忤物，亦不隨流，真所謂鞠躬君子者矣。夙惠之性，稟于天資。年十餘歲，侍伯父食，不過園疏而已。伯父戲之曰：‘啜白薤之羹，淡而無味。’君應聲答曰：‘齧紫茄之蔕，鏗爾有聲。’人知其當大成也。余始聞其名，晚乃識面，察言觀行，重其爲人。藩房見選，余所薦也，亦既稱職，頗嘗自多。丙寅歲與君俱年五十歲，日會飲酒，相與賦詩，君先就，曰：‘學《易》寧無道?知非素有心。’余遂不復作也。君有文集二十卷。嗚呼!契闊夷險，咨嗟年鬢，一生一死，孰克忘情!聊存掛劍之期，故有刊銘之作。其詞曰：嗚呼江君，世濟其名。生今之俗，爲古之人。閨門侃侃，鄉里恂恂。其實如秋，其華如春。握蘭有裕，伏閣惟勤。考終歸全，邈焉清塵。葬于所沒，古稱達者。浚水長源，夷門迥野。徒掛寶劍，空馳白馬。勝氣如存，逝川不捨。勒石垂芳，千載之下。《徐公文集》卷二九。〔一〕辟：原作‘辭’，據徐校、李刊本改。</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>9</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>太常寺奉禮郎;太常寺奉禮郎;縣令;江夏;縣令;黃梅;縣令;縣主簿;江都</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>太平興國</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>15;宋</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1762</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1762</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>王安石</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>進士</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>進士舉人測試</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
         <is>
           <t>15;宋</t>
         </is>

</xml_diff>

<commit_message>
update the algrithum to calculate biogaddr scores
</commit_message>
<xml_diff>
--- a/compare-result-list.xlsx
+++ b/compare-result-list.xlsx
@@ -1236,7 +1236,7 @@
         <v>27</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1245,7 +1245,7 @@
         <v>37</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
create functions for only_zero_score column
</commit_message>
<xml_diff>
--- a/compare-result-list.xlsx
+++ b/compare-result-list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
   <si>
     <t>input_id</t>
   </si>
@@ -290,6 +290,15 @@
   </si>
   <si>
     <t>18;元</t>
+  </si>
+  <si>
+    <t>only_zero_score</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -621,13 +630,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,8 +691,11 @@
       <c r="R1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -723,8 +735,11 @@
       <c r="R2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="T2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -764,8 +779,11 @@
       <c r="R3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="T3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -814,8 +832,11 @@
       <c r="R4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="T4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -852,8 +873,11 @@
       <c r="R5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="T5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -890,8 +914,11 @@
       <c r="R6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="T6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -928,8 +955,11 @@
       <c r="R7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="T7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -975,8 +1005,11 @@
       <c r="R8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="T8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1013,8 +1046,11 @@
       <c r="R9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="T9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1051,8 +1087,11 @@
       <c r="R10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="T10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1095,8 +1134,11 @@
       <c r="R11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="T11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1133,8 +1175,11 @@
       <c r="R12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="T12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1171,8 +1216,11 @@
       <c r="R13" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="T13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1224,8 +1272,11 @@
       <c r="R14" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="T14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1274,8 +1325,11 @@
       <c r="R15" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="T15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1312,8 +1366,11 @@
       <c r="R16" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="T16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1350,8 +1407,11 @@
       <c r="R17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="T17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1391,8 +1451,11 @@
       <c r="R18" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="T18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1429,8 +1492,11 @@
       <c r="R19" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="T19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1467,8 +1533,11 @@
       <c r="R20" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="T20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1514,8 +1583,11 @@
       <c r="R21" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="T21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1561,8 +1633,11 @@
       <c r="R22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="T22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1601,6 +1676,9 @@
       </c>
       <c r="R23" t="s">
         <v>90</v>
+      </c>
+      <c r="T23" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean writing titles before match
</commit_message>
<xml_diff>
--- a/compare-result-list.xlsx
+++ b/compare-result-list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>比部員外郎;給事中;宣州;翰林學士;判太常卿事;水部員外郎;衛尉卿;營田副使;江州;右諫議大夫;御史中丞;知制誥;主客郎中;司士參軍;江州</t>
+          <t>比部員外郎;給事中;宣州;翰林學士;判太常卿事;水部員外郎;衛尉卿;營田副使;江州;右諫議大夫;御史中丞;知制誥;司士參軍;江州;主客郎中</t>
         </is>
       </c>
       <c r="N4" t="n">
@@ -999,7 +999,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>祠部郎中;大理評事;殿中監;給事中;駕部員外郎;秘書省正字;司農少卿;水部員外郎;屯田員外郎;修國史;刑部侍郎;知制誥;中書舍人</t>
+          <t>祠部郎中;大理評事;殿中監;給事中;駕部員外郎;秘書省正字;水部員外郎;司農少卿;屯田員外郎;修國史;刑部侍郎;知制誥;中書舍人</t>
         </is>
       </c>
       <c r="N8" t="n">
@@ -1949,7 +1949,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -1997,9 +1997,13 @@
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="n">
-        <v>0</v>
-      </c>
-      <c r="U22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>文集</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr">
         <is>
           <t>15;宋</t>
@@ -2083,6 +2087,213 @@
         </is>
       </c>
       <c r="W23" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11833</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>11833</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>劉玶</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>有詩集存世</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="n">
+        <v>1</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>詩集</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>15;宋</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10111</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>10111</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>唐慎微</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>重修政和經史證類備用本草</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>經史證類備用本草</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>15;宋</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10831</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>10831</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>李心傳</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>著建炎以來朝野雜記</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="n">
+        <v>1</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>以來朝野雜記</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>15;宋</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
         <is>
           <t>no</t>
         </is>

</xml_diff>

<commit_message>
clean source text before match
</commit_message>
<xml_diff>
--- a/compare-result-list.xlsx
+++ b/compare-result-list.xlsx
@@ -2233,15 +2233,15 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10831</t>
+          <t>51241</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>10831</v>
+        <v>51241</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>李心傳</t>
+          <t>鄭涇</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2261,7 +2261,7 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>著建炎以來朝野雜記</t>
+          <t>見登科錄</t>
         </is>
       </c>
       <c r="L26" t="n">
@@ -2277,17 +2277,17 @@
       </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
-        <v>0</v>
-      </c>
-      <c r="S26" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>登科錄</t>
+        </is>
+      </c>
       <c r="T26" t="n">
-        <v>1</v>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>以來朝野雜記</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr">
         <is>
           <t>15;宋</t>

</xml_diff>